<commit_message>
Membuat Profile, Timeline, Hoshin Kanry, KPI Performance
</commit_message>
<xml_diff>
--- a/Data-Data/Laporan KPI GR 2020 Auto2000 Banyuwangi.xlsx
+++ b/Data-Data/Laporan KPI GR 2020 Auto2000 Banyuwangi.xlsx
@@ -1,35 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT_WIndows\Kaizen2021\Data-Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AB47A-9BCD-4FD6-9A15-773DAC109DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="5" r:id="rId1"/>
     <sheet name="KPI A2000 Banyuwangi" sheetId="12" r:id="rId2"/>
-    <sheet name="by model (A2000 Banyuwangi)" sheetId="13" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId3"/>
+    <sheet name="by model (A2000 Banyuwangi)" sheetId="13" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'by model (A2000 Banyuwangi)'!$A$1:$AE$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'by model (A2000 Banyuwangi)'!$A$1:$AE$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Guidance!$B$1:$U$177</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'KPI A2000 Banyuwangi'!$B$1:$T$148</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>faozan035906</author>
   </authors>
   <commentList>
-    <comment ref="I95" authorId="0">
+    <comment ref="I95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J95" authorId="0">
+    <comment ref="J95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K95" authorId="0">
+    <comment ref="K95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L95" authorId="0">
+    <comment ref="L95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -141,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M95" authorId="0">
+    <comment ref="M95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N95" authorId="0">
+    <comment ref="N95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -197,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O95" authorId="0">
+    <comment ref="O95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P95" authorId="0">
+    <comment ref="P95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q95" authorId="0">
+    <comment ref="Q95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -281,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R95" authorId="0">
+    <comment ref="R95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="421">
   <si>
     <t>BRANCH_NAME</t>
   </si>
@@ -1739,11 +1746,104 @@
   <si>
     <t>11.0</t>
   </si>
+  <si>
+    <t>Return Job</t>
+  </si>
+  <si>
+    <t>RTJ Rate</t>
+  </si>
+  <si>
+    <t>PSFU</t>
+  </si>
+  <si>
+    <t>jumlah total ue yang di PSFU</t>
+  </si>
+  <si>
+    <t>Unet Entry</t>
+  </si>
+  <si>
+    <t>Succes Call PSFU</t>
+  </si>
+  <si>
+    <t>Succes Call PSFU Rate</t>
+  </si>
+  <si>
+    <t>LEADTIME</t>
+  </si>
+  <si>
+    <t>Ledtime Total</t>
+  </si>
+  <si>
+    <t>Target Leadtime Total</t>
+  </si>
+  <si>
+    <t>Leadtime SBE</t>
+  </si>
+  <si>
+    <t>Target Leadtime SBE</t>
+  </si>
+  <si>
+    <t>Achievement</t>
+  </si>
+  <si>
+    <t>Leadtime EM</t>
+  </si>
+  <si>
+    <t>Target Leadtime EM</t>
+  </si>
+  <si>
+    <t>ONTIME DELIVERY</t>
+  </si>
+  <si>
+    <t>1st Promise</t>
+  </si>
+  <si>
+    <t>1st Promise rate (%)</t>
+  </si>
+  <si>
+    <t>EXPRESS MAINTENANCE</t>
+  </si>
+  <si>
+    <t>unit EM</t>
+  </si>
+  <si>
+    <t>% EM</t>
+  </si>
+  <si>
+    <t>Unit SBE</t>
+  </si>
+  <si>
+    <t>APPOINMENT</t>
+  </si>
+  <si>
+    <t>Jumlah booking</t>
+  </si>
+  <si>
+    <t>App. Rate</t>
+  </si>
+  <si>
+    <t>CPUS</t>
+  </si>
+  <si>
+    <t>CPUS Rate</t>
+  </si>
+  <si>
+    <t>SBI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBI Total </t>
+  </si>
+  <si>
+    <t>SBI Same Outlet</t>
+  </si>
+  <si>
+    <t>SBI Same Outlet (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -1755,7 +1855,7 @@
     <numFmt numFmtId="169" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1937,6 +2037,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2845,7 +2953,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="655">
+  <cellXfs count="659">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -4794,12 +4902,63 @@
     <xf numFmtId="170" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4821,24 +4980,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4851,38 +4992,50 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="41" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="42" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="43" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="25" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="26" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="30" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="31" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="11" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="12" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -4929,80 +5082,39 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="41" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="42" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="43" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="25" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="26" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="30" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="31" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="11" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="12" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="AutoFormat-Optionen" xfId="18"/>
+    <cellStyle name="AutoFormat-Optionen" xfId="18" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Comma [0] 2" xfId="12"/>
-    <cellStyle name="Comma 10" xfId="17"/>
-    <cellStyle name="Comma 10 2" xfId="25"/>
-    <cellStyle name="Comma 2" xfId="4"/>
-    <cellStyle name="Comma 2 2" xfId="13"/>
-    <cellStyle name="Comma 2 3" xfId="24"/>
-    <cellStyle name="Comma 3" xfId="19"/>
-    <cellStyle name="Comma 4" xfId="5"/>
-    <cellStyle name="Comma 5" xfId="14"/>
-    <cellStyle name="Comma 7" xfId="20"/>
-    <cellStyle name="Excel Built-in Comma" xfId="15"/>
-    <cellStyle name="Excel Built-in Normal" xfId="11"/>
-    <cellStyle name="Excel Built-in Percent" xfId="16"/>
+    <cellStyle name="Comma [0] 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 10" xfId="17" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 10 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 2 3" xfId="24" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Comma 4" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Comma 5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Comma 7" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Excel Built-in Comma" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="11" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Excel Built-in Percent" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 12 2" xfId="21"/>
-    <cellStyle name="Normal 2" xfId="22"/>
-    <cellStyle name="Normal 3" xfId="26"/>
-    <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 5" xfId="9"/>
-    <cellStyle name="Normal 8" xfId="23"/>
+    <cellStyle name="Normal 12 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 3" xfId="26" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 8" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="6"/>
-    <cellStyle name="Percent 3" xfId="10"/>
-    <cellStyle name="Percent 4" xfId="8"/>
+    <cellStyle name="Percent 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Percent 3" xfId="10" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Percent 4" xfId="8" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5034,7 +5146,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3"/>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5095,7 +5213,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5209,7 +5333,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -5218,7 +5348,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5238,7 +5368,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -5264,7 +5394,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5359,7 +5495,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5454,7 +5596,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5568,7 +5716,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -5671,7 +5825,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="DATA BANK"/>
@@ -5809,7 +5963,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5841,9 +5995,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5875,6 +6047,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6050,7 +6240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6118,8 +6308,8 @@
       </c>
       <c r="C3" s="100"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="614"/>
-      <c r="F3" s="614"/>
+      <c r="E3" s="609"/>
+      <c r="F3" s="609"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -6137,8 +6327,8 @@
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="31"/>
-      <c r="E4" s="614"/>
-      <c r="F4" s="614"/>
+      <c r="E4" s="609"/>
+      <c r="F4" s="609"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -6175,12 +6365,12 @@
       <c r="B6" s="206" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="615" t="s">
+      <c r="C6" s="610" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="616"/>
-      <c r="E6" s="616"/>
-      <c r="F6" s="617"/>
+      <c r="D6" s="611"/>
+      <c r="E6" s="611"/>
+      <c r="F6" s="612"/>
       <c r="G6" s="206"/>
       <c r="H6" s="224" t="s">
         <v>137</v>
@@ -6251,11 +6441,11 @@
     <row r="8" spans="1:21" s="37" customFormat="1">
       <c r="B8" s="278"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="604" t="s">
+      <c r="D8" s="598" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="605"/>
-      <c r="F8" s="606"/>
+      <c r="E8" s="599"/>
+      <c r="F8" s="600"/>
       <c r="G8" s="49"/>
       <c r="H8" s="177"/>
       <c r="I8" s="177"/>
@@ -6298,7 +6488,7 @@
       <c r="R9" s="56"/>
       <c r="S9" s="56"/>
       <c r="T9" s="43"/>
-      <c r="U9" s="597" t="s">
+      <c r="U9" s="614" t="s">
         <v>227</v>
       </c>
     </row>
@@ -6328,16 +6518,16 @@
       <c r="R10" s="56"/>
       <c r="S10" s="56"/>
       <c r="T10" s="43"/>
-      <c r="U10" s="597"/>
+      <c r="U10" s="614"/>
     </row>
     <row r="11" spans="1:21" s="37" customFormat="1">
       <c r="B11" s="278"/>
       <c r="C11" s="33"/>
-      <c r="D11" s="604" t="s">
+      <c r="D11" s="598" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="605"/>
-      <c r="F11" s="606"/>
+      <c r="E11" s="599"/>
+      <c r="F11" s="600"/>
       <c r="G11" s="51"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -6380,7 +6570,7 @@
       <c r="R12" s="56"/>
       <c r="S12" s="56"/>
       <c r="T12" s="43"/>
-      <c r="U12" s="597" t="s">
+      <c r="U12" s="614" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6410,7 +6600,7 @@
       <c r="R13" s="56"/>
       <c r="S13" s="56"/>
       <c r="T13" s="43"/>
-      <c r="U13" s="597"/>
+      <c r="U13" s="614"/>
     </row>
     <row r="14" spans="1:21" s="37" customFormat="1">
       <c r="B14" s="278"/>
@@ -6462,7 +6652,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
       <c r="T15" s="245"/>
-      <c r="U15" s="597" t="s">
+      <c r="U15" s="614" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6492,7 +6682,7 @@
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
       <c r="T16" s="245"/>
-      <c r="U16" s="597"/>
+      <c r="U16" s="614"/>
     </row>
     <row r="17" spans="1:23" s="47" customFormat="1">
       <c r="A17" s="37"/>
@@ -6553,10 +6743,10 @@
     <row r="19" spans="1:23" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B19" s="278"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="604" t="s">
+      <c r="D19" s="598" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="618"/>
+      <c r="E19" s="613"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="H19" s="177"/>
@@ -6730,10 +6920,10 @@
     <row r="24" spans="1:23" ht="13.15" customHeight="1">
       <c r="B24" s="278"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="598" t="s">
+      <c r="D24" s="615" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="601" t="s">
+      <c r="E24" s="618" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
@@ -6762,8 +6952,8 @@
     <row r="25" spans="1:23" ht="13.15" customHeight="1">
       <c r="B25" s="278"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="599"/>
-      <c r="E25" s="602"/>
+      <c r="D25" s="616"/>
+      <c r="E25" s="619"/>
       <c r="F25" s="18" t="s">
         <v>253</v>
       </c>
@@ -6790,8 +6980,8 @@
     <row r="26" spans="1:23">
       <c r="B26" s="278"/>
       <c r="C26" s="33"/>
-      <c r="D26" s="599"/>
-      <c r="E26" s="602"/>
+      <c r="D26" s="616"/>
+      <c r="E26" s="619"/>
       <c r="F26" s="18" t="s">
         <v>254</v>
       </c>
@@ -6819,8 +7009,8 @@
     <row r="27" spans="1:23" ht="13.15" customHeight="1">
       <c r="B27" s="278"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="599"/>
-      <c r="E27" s="602"/>
+      <c r="D27" s="616"/>
+      <c r="E27" s="619"/>
       <c r="F27" s="18" t="s">
         <v>255</v>
       </c>
@@ -6847,8 +7037,8 @@
     <row r="28" spans="1:23" ht="13.15" customHeight="1">
       <c r="B28" s="278"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="599"/>
-      <c r="E28" s="602"/>
+      <c r="D28" s="616"/>
+      <c r="E28" s="619"/>
       <c r="F28" s="18" t="s">
         <v>256</v>
       </c>
@@ -6877,8 +7067,8 @@
     <row r="29" spans="1:23" ht="13.15" customHeight="1">
       <c r="B29" s="278"/>
       <c r="C29" s="33"/>
-      <c r="D29" s="599"/>
-      <c r="E29" s="602"/>
+      <c r="D29" s="616"/>
+      <c r="E29" s="619"/>
       <c r="F29" s="18" t="s">
         <v>257</v>
       </c>
@@ -6907,8 +7097,8 @@
     <row r="30" spans="1:23" ht="13.15" customHeight="1">
       <c r="B30" s="278"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="599"/>
-      <c r="E30" s="602"/>
+      <c r="D30" s="616"/>
+      <c r="E30" s="619"/>
       <c r="F30" s="18" t="s">
         <v>258</v>
       </c>
@@ -6937,8 +7127,8 @@
     <row r="31" spans="1:23" ht="13.15" customHeight="1">
       <c r="B31" s="278"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="599"/>
-      <c r="E31" s="602"/>
+      <c r="D31" s="616"/>
+      <c r="E31" s="619"/>
       <c r="F31" s="18" t="s">
         <v>259</v>
       </c>
@@ -6967,8 +7157,8 @@
     <row r="32" spans="1:23" ht="13.15" customHeight="1">
       <c r="B32" s="278"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="599"/>
-      <c r="E32" s="602"/>
+      <c r="D32" s="616"/>
+      <c r="E32" s="619"/>
       <c r="F32" s="18" t="s">
         <v>260</v>
       </c>
@@ -6998,8 +7188,8 @@
     <row r="33" spans="1:21" ht="13.15" customHeight="1">
       <c r="B33" s="278"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="599"/>
-      <c r="E33" s="602"/>
+      <c r="D33" s="616"/>
+      <c r="E33" s="619"/>
       <c r="F33" s="18" t="s">
         <v>261</v>
       </c>
@@ -7025,8 +7215,8 @@
     <row r="34" spans="1:21" ht="13.15" customHeight="1">
       <c r="B34" s="278"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="599"/>
-      <c r="E34" s="602"/>
+      <c r="D34" s="616"/>
+      <c r="E34" s="619"/>
       <c r="F34" s="28" t="s">
         <v>19</v>
       </c>
@@ -7055,8 +7245,8 @@
     <row r="35" spans="1:21" ht="13.15" customHeight="1">
       <c r="B35" s="278"/>
       <c r="C35" s="33"/>
-      <c r="D35" s="599"/>
-      <c r="E35" s="603"/>
+      <c r="D35" s="616"/>
+      <c r="E35" s="620"/>
       <c r="F35" s="31" t="s">
         <v>20</v>
       </c>
@@ -7083,7 +7273,7 @@
     <row r="36" spans="1:21" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B36" s="278"/>
       <c r="C36" s="33"/>
-      <c r="D36" s="600"/>
+      <c r="D36" s="617"/>
       <c r="E36" s="34" t="s">
         <v>125</v>
       </c>
@@ -7148,7 +7338,7 @@
     <row r="37" spans="1:21" ht="13.15" customHeight="1">
       <c r="B37" s="278"/>
       <c r="C37" s="33"/>
-      <c r="D37" s="607" t="s">
+      <c r="D37" s="603" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="58" t="s">
@@ -7179,7 +7369,7 @@
     <row r="38" spans="1:21" ht="13.15" customHeight="1">
       <c r="B38" s="278"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="608"/>
+      <c r="D38" s="604"/>
       <c r="E38" s="28" t="s">
         <v>23</v>
       </c>
@@ -7210,7 +7400,7 @@
     <row r="39" spans="1:21" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B39" s="278"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="609"/>
+      <c r="D39" s="605"/>
       <c r="E39" s="34" t="s">
         <v>126</v>
       </c>
@@ -7300,10 +7490,10 @@
     <row r="41" spans="1:21" ht="13.15" customHeight="1">
       <c r="B41" s="278"/>
       <c r="C41" s="33"/>
-      <c r="D41" s="610" t="s">
+      <c r="D41" s="621" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="611"/>
+      <c r="E41" s="622"/>
       <c r="F41" s="31" t="s">
         <v>262</v>
       </c>
@@ -7330,8 +7520,8 @@
     <row r="42" spans="1:21" ht="13.15" customHeight="1">
       <c r="B42" s="278"/>
       <c r="C42" s="33"/>
-      <c r="D42" s="612"/>
-      <c r="E42" s="613"/>
+      <c r="D42" s="623"/>
+      <c r="E42" s="624"/>
       <c r="F42" s="31" t="s">
         <v>263</v>
       </c>
@@ -7361,10 +7551,10 @@
     <row r="43" spans="1:21" ht="13.15" customHeight="1">
       <c r="B43" s="278"/>
       <c r="C43" s="33"/>
-      <c r="D43" s="595" t="s">
+      <c r="D43" s="596" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="596"/>
+      <c r="E43" s="597"/>
       <c r="F43" s="31"/>
       <c r="G43" s="274">
         <v>29</v>
@@ -7389,10 +7579,10 @@
     <row r="44" spans="1:21" ht="13.15" customHeight="1">
       <c r="B44" s="278"/>
       <c r="C44" s="33"/>
-      <c r="D44" s="595" t="s">
+      <c r="D44" s="596" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="596"/>
+      <c r="E44" s="597"/>
       <c r="F44" s="31"/>
       <c r="G44" s="274">
         <v>30</v>
@@ -7417,10 +7607,10 @@
     <row r="45" spans="1:21" ht="13.15" customHeight="1">
       <c r="B45" s="278"/>
       <c r="C45" s="33"/>
-      <c r="D45" s="595" t="s">
+      <c r="D45" s="596" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="596"/>
+      <c r="E45" s="597"/>
       <c r="F45" s="31"/>
       <c r="G45" s="274">
         <v>31</v>
@@ -7593,7 +7783,7 @@
     <row r="50" spans="1:21">
       <c r="B50" s="278"/>
       <c r="C50" s="33"/>
-      <c r="D50" s="607" t="s">
+      <c r="D50" s="603" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="74" t="s">
@@ -7626,7 +7816,7 @@
     <row r="51" spans="1:21">
       <c r="B51" s="278"/>
       <c r="C51" s="33"/>
-      <c r="D51" s="608"/>
+      <c r="D51" s="604"/>
       <c r="E51" s="74" t="s">
         <v>36</v>
       </c>
@@ -7657,7 +7847,7 @@
     <row r="52" spans="1:21">
       <c r="B52" s="278"/>
       <c r="C52" s="33"/>
-      <c r="D52" s="608"/>
+      <c r="D52" s="604"/>
       <c r="E52" s="74" t="s">
         <v>37</v>
       </c>
@@ -7688,7 +7878,7 @@
     <row r="53" spans="1:21">
       <c r="B53" s="278"/>
       <c r="C53" s="33"/>
-      <c r="D53" s="608"/>
+      <c r="D53" s="604"/>
       <c r="E53" s="74" t="s">
         <v>38</v>
       </c>
@@ -7719,7 +7909,7 @@
     <row r="54" spans="1:21" s="37" customFormat="1" ht="13.5" thickBot="1">
       <c r="B54" s="278"/>
       <c r="C54" s="84"/>
-      <c r="D54" s="609"/>
+      <c r="D54" s="605"/>
       <c r="E54" s="170" t="s">
         <v>128</v>
       </c>
@@ -7870,7 +8060,7 @@
     <row r="58" spans="1:21">
       <c r="B58" s="278"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="623" t="s">
+      <c r="D58" s="607" t="s">
         <v>43</v>
       </c>
       <c r="E58" s="86" t="s">
@@ -7903,7 +8093,7 @@
     <row r="59" spans="1:21">
       <c r="B59" s="278"/>
       <c r="C59" s="33"/>
-      <c r="D59" s="623"/>
+      <c r="D59" s="607"/>
       <c r="E59" s="86" t="s">
         <v>45</v>
       </c>
@@ -7935,7 +8125,7 @@
       <c r="A60" s="285"/>
       <c r="B60" s="278"/>
       <c r="C60" s="33"/>
-      <c r="D60" s="623"/>
+      <c r="D60" s="607"/>
       <c r="E60" s="34" t="s">
         <v>87</v>
       </c>
@@ -8003,7 +8193,7 @@
     <row r="61" spans="1:21">
       <c r="B61" s="278"/>
       <c r="C61" s="230"/>
-      <c r="D61" s="623"/>
+      <c r="D61" s="607"/>
       <c r="E61" s="86" t="s">
         <v>104</v>
       </c>
@@ -8034,7 +8224,7 @@
     <row r="62" spans="1:21">
       <c r="B62" s="278"/>
       <c r="C62" s="33"/>
-      <c r="D62" s="623"/>
+      <c r="D62" s="607"/>
       <c r="E62" s="86" t="s">
         <v>103</v>
       </c>
@@ -8155,11 +8345,11 @@
     <row r="65" spans="1:21">
       <c r="B65" s="278"/>
       <c r="C65" s="33"/>
-      <c r="D65" s="619" t="s">
+      <c r="D65" s="595" t="s">
         <v>94</v>
       </c>
-      <c r="E65" s="619"/>
-      <c r="F65" s="619"/>
+      <c r="E65" s="595"/>
+      <c r="F65" s="595"/>
       <c r="G65" s="274">
         <v>46</v>
       </c>
@@ -8185,11 +8375,11 @@
     <row r="66" spans="1:21">
       <c r="B66" s="278"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="619" t="s">
+      <c r="D66" s="595" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="619"/>
-      <c r="F66" s="619"/>
+      <c r="E66" s="595"/>
+      <c r="F66" s="595"/>
       <c r="G66" s="274">
         <v>47</v>
       </c>
@@ -8239,11 +8429,11 @@
     <row r="68" spans="1:21">
       <c r="B68" s="278"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="619" t="s">
+      <c r="D68" s="595" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="619"/>
-      <c r="F68" s="619"/>
+      <c r="E68" s="595"/>
+      <c r="F68" s="595"/>
       <c r="G68" s="274">
         <v>48</v>
       </c>
@@ -8269,11 +8459,11 @@
     <row r="69" spans="1:21">
       <c r="B69" s="278"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="619" t="s">
+      <c r="D69" s="595" t="s">
         <v>122</v>
       </c>
-      <c r="E69" s="619"/>
-      <c r="F69" s="619"/>
+      <c r="E69" s="595"/>
+      <c r="F69" s="595"/>
       <c r="G69" s="274">
         <v>49</v>
       </c>
@@ -8299,11 +8489,11 @@
     <row r="70" spans="1:21">
       <c r="B70" s="278"/>
       <c r="C70" s="33"/>
-      <c r="D70" s="619" t="s">
+      <c r="D70" s="595" t="s">
         <v>123</v>
       </c>
-      <c r="E70" s="619"/>
-      <c r="F70" s="619"/>
+      <c r="E70" s="595"/>
+      <c r="F70" s="595"/>
       <c r="G70" s="274">
         <v>50</v>
       </c>
@@ -8353,7 +8543,7 @@
     <row r="72" spans="1:21">
       <c r="B72" s="278"/>
       <c r="C72" s="33"/>
-      <c r="D72" s="624" t="s">
+      <c r="D72" s="608" t="s">
         <v>46</v>
       </c>
       <c r="E72" s="98" t="s">
@@ -8385,7 +8575,7 @@
     <row r="73" spans="1:21">
       <c r="B73" s="278"/>
       <c r="C73" s="33"/>
-      <c r="D73" s="624"/>
+      <c r="D73" s="608"/>
       <c r="E73" s="98" t="s">
         <v>105</v>
       </c>
@@ -8416,7 +8606,7 @@
     <row r="74" spans="1:21">
       <c r="B74" s="278"/>
       <c r="C74" s="33"/>
-      <c r="D74" s="624"/>
+      <c r="D74" s="608"/>
       <c r="E74" s="98" t="s">
         <v>48</v>
       </c>
@@ -8447,7 +8637,7 @@
     <row r="75" spans="1:21">
       <c r="B75" s="278"/>
       <c r="C75" s="33"/>
-      <c r="D75" s="624"/>
+      <c r="D75" s="608"/>
       <c r="E75" s="98" t="s">
         <v>49</v>
       </c>
@@ -8478,7 +8668,7 @@
     <row r="76" spans="1:21">
       <c r="B76" s="278"/>
       <c r="C76" s="33"/>
-      <c r="D76" s="624"/>
+      <c r="D76" s="608"/>
       <c r="E76" s="98" t="s">
         <v>50</v>
       </c>
@@ -8509,7 +8699,7 @@
     <row r="77" spans="1:21">
       <c r="B77" s="278"/>
       <c r="C77" s="33"/>
-      <c r="D77" s="624"/>
+      <c r="D77" s="608"/>
       <c r="E77" s="74" t="s">
         <v>51</v>
       </c>
@@ -8677,7 +8867,7 @@
     <row r="80" spans="1:21">
       <c r="B80" s="278"/>
       <c r="C80" s="33"/>
-      <c r="D80" s="607" t="s">
+      <c r="D80" s="603" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="98" t="s">
@@ -8709,7 +8899,7 @@
     <row r="81" spans="2:21">
       <c r="B81" s="278"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="608"/>
+      <c r="D81" s="604"/>
       <c r="E81" s="98" t="s">
         <v>201</v>
       </c>
@@ -8740,7 +8930,7 @@
     <row r="82" spans="2:21">
       <c r="B82" s="278"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="608"/>
+      <c r="D82" s="604"/>
       <c r="E82" s="98" t="s">
         <v>202</v>
       </c>
@@ -8771,7 +8961,7 @@
     <row r="83" spans="2:21">
       <c r="B83" s="278"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="609"/>
+      <c r="D83" s="605"/>
       <c r="E83" s="98" t="s">
         <v>203</v>
       </c>
@@ -8870,13 +9060,13 @@
     <row r="85" spans="2:21" ht="13.15" customHeight="1">
       <c r="B85" s="278"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="622" t="s">
+      <c r="D85" s="606" t="s">
         <v>53</v>
       </c>
-      <c r="E85" s="595" t="s">
+      <c r="E85" s="596" t="s">
         <v>206</v>
       </c>
-      <c r="F85" s="596"/>
+      <c r="F85" s="597"/>
       <c r="G85" s="274">
         <f t="shared" si="11"/>
         <v>64</v>
@@ -8903,7 +9093,7 @@
     <row r="86" spans="2:21">
       <c r="B86" s="278"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="622"/>
+      <c r="D86" s="606"/>
       <c r="E86" s="98" t="s">
         <v>54</v>
       </c>
@@ -8934,7 +9124,7 @@
     <row r="87" spans="2:21">
       <c r="B87" s="278"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="622"/>
+      <c r="D87" s="606"/>
       <c r="E87" s="34" t="s">
         <v>134</v>
       </c>
@@ -9002,7 +9192,7 @@
     <row r="88" spans="2:21">
       <c r="B88" s="278"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="622" t="s">
+      <c r="D88" s="606" t="s">
         <v>55</v>
       </c>
       <c r="E88" s="98" t="s">
@@ -9035,7 +9225,7 @@
     <row r="89" spans="2:21">
       <c r="B89" s="278"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="622"/>
+      <c r="D89" s="606"/>
       <c r="E89" s="98" t="s">
         <v>56</v>
       </c>
@@ -9066,7 +9256,7 @@
     <row r="90" spans="2:21">
       <c r="B90" s="278"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="622"/>
+      <c r="D90" s="606"/>
       <c r="E90" s="98" t="s">
         <v>200</v>
       </c>
@@ -9097,7 +9287,7 @@
     <row r="91" spans="2:21">
       <c r="B91" s="278"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="607" t="s">
+      <c r="D91" s="603" t="s">
         <v>57</v>
       </c>
       <c r="E91" s="98" t="s">
@@ -9130,7 +9320,7 @@
     <row r="92" spans="2:21" s="102" customFormat="1">
       <c r="B92" s="278"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="608"/>
+      <c r="D92" s="604"/>
       <c r="E92" s="98" t="s">
         <v>58</v>
       </c>
@@ -9161,7 +9351,7 @@
     <row r="93" spans="2:21">
       <c r="B93" s="278"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="609"/>
+      <c r="D93" s="605"/>
       <c r="E93" s="98" t="s">
         <v>207</v>
       </c>
@@ -9260,11 +9450,11 @@
     <row r="95" spans="2:21">
       <c r="B95" s="278"/>
       <c r="C95" s="84"/>
-      <c r="D95" s="604" t="s">
+      <c r="D95" s="598" t="s">
         <v>59</v>
       </c>
-      <c r="E95" s="605"/>
-      <c r="F95" s="606"/>
+      <c r="E95" s="599"/>
+      <c r="F95" s="600"/>
       <c r="G95" s="274">
         <f t="shared" si="11"/>
         <v>74</v>
@@ -10308,8 +10498,8 @@
         <v>79</v>
       </c>
       <c r="D125" s="148"/>
-      <c r="E125" s="620"/>
-      <c r="F125" s="621"/>
+      <c r="E125" s="601"/>
+      <c r="F125" s="602"/>
       <c r="G125" s="274"/>
       <c r="H125" s="226"/>
       <c r="I125" s="147"/>
@@ -11896,6 +12086,21 @@
     <protectedRange sqref="H100:H104 H111:H114 H106:H107" name="Range17_1_1_1_8_1"/>
   </protectedRanges>
   <mergeCells count="31">
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="U15:U16"/>
+    <mergeCell ref="D24:D36"/>
+    <mergeCell ref="E24:E35"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D69:F69"/>
     <mergeCell ref="D70:F70"/>
     <mergeCell ref="D45:E45"/>
@@ -11912,39 +12117,24 @@
     <mergeCell ref="D72:D77"/>
     <mergeCell ref="D65:F65"/>
     <mergeCell ref="D68:F68"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="U12:U13"/>
-    <mergeCell ref="U15:U16"/>
-    <mergeCell ref="D24:D36"/>
-    <mergeCell ref="E24:E35"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="D41:E42"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="52" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="53" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft" activeCell="P144" sqref="P144:Q144"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41:R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -11995,8 +12185,8 @@
       </c>
       <c r="C3" s="100"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="614"/>
-      <c r="F3" s="614"/>
+      <c r="E3" s="609"/>
+      <c r="F3" s="609"/>
       <c r="H3" s="182"/>
       <c r="I3" s="182"/>
       <c r="J3" s="182"/>
@@ -12010,8 +12200,8 @@
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="31"/>
-      <c r="E4" s="614"/>
-      <c r="F4" s="614"/>
+      <c r="E4" s="609"/>
+      <c r="F4" s="609"/>
       <c r="H4" s="355"/>
       <c r="I4" s="355"/>
       <c r="J4" s="355"/>
@@ -12047,12 +12237,12 @@
       <c r="B6" s="206" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="615" t="s">
+      <c r="C6" s="610" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="616"/>
-      <c r="E6" s="616"/>
-      <c r="F6" s="617"/>
+      <c r="D6" s="611"/>
+      <c r="E6" s="611"/>
+      <c r="F6" s="612"/>
       <c r="G6" s="206"/>
       <c r="H6" s="224" t="s">
         <v>137</v>
@@ -12122,11 +12312,11 @@
     <row r="8" spans="1:20" s="37" customFormat="1">
       <c r="B8" s="278"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="604" t="s">
+      <c r="D8" s="598" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="605"/>
-      <c r="F8" s="606"/>
+      <c r="E8" s="599"/>
+      <c r="F8" s="600"/>
       <c r="G8" s="49"/>
       <c r="H8" s="361"/>
       <c r="I8" s="361"/>
@@ -12239,11 +12429,11 @@
     <row r="11" spans="1:20" s="37" customFormat="1">
       <c r="B11" s="278"/>
       <c r="C11" s="33"/>
-      <c r="D11" s="604" t="s">
+      <c r="D11" s="598" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="605"/>
-      <c r="F11" s="606"/>
+      <c r="E11" s="599"/>
+      <c r="F11" s="600"/>
       <c r="G11" s="51"/>
       <c r="H11" s="366"/>
       <c r="I11" s="366"/>
@@ -12545,10 +12735,10 @@
     <row r="19" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B19" s="278"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="604" t="s">
+      <c r="D19" s="598" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="618"/>
+      <c r="E19" s="613"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="H19" s="361"/>
@@ -12749,10 +12939,10 @@
     <row r="24" spans="1:20" ht="13.15" customHeight="1">
       <c r="B24" s="278"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="598" t="s">
+      <c r="D24" s="615" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="601" t="s">
+      <c r="E24" s="618" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
@@ -12800,8 +12990,8 @@
     <row r="25" spans="1:20" ht="13.15" customHeight="1">
       <c r="B25" s="278"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="599"/>
-      <c r="E25" s="602"/>
+      <c r="D25" s="616"/>
+      <c r="E25" s="619"/>
       <c r="F25" s="18" t="s">
         <v>253</v>
       </c>
@@ -12847,8 +13037,8 @@
     <row r="26" spans="1:20">
       <c r="B26" s="278"/>
       <c r="C26" s="33"/>
-      <c r="D26" s="599"/>
-      <c r="E26" s="602"/>
+      <c r="D26" s="616"/>
+      <c r="E26" s="619"/>
       <c r="F26" s="18" t="s">
         <v>254</v>
       </c>
@@ -12895,8 +13085,8 @@
     <row r="27" spans="1:20" ht="13.15" customHeight="1">
       <c r="B27" s="278"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="599"/>
-      <c r="E27" s="602"/>
+      <c r="D27" s="616"/>
+      <c r="E27" s="619"/>
       <c r="F27" s="18" t="s">
         <v>255</v>
       </c>
@@ -12942,8 +13132,8 @@
     <row r="28" spans="1:20" ht="13.15" customHeight="1">
       <c r="B28" s="278"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="599"/>
-      <c r="E28" s="602"/>
+      <c r="D28" s="616"/>
+      <c r="E28" s="619"/>
       <c r="F28" s="18" t="s">
         <v>256</v>
       </c>
@@ -12989,8 +13179,8 @@
     <row r="29" spans="1:20" ht="13.15" customHeight="1">
       <c r="B29" s="278"/>
       <c r="C29" s="33"/>
-      <c r="D29" s="599"/>
-      <c r="E29" s="602"/>
+      <c r="D29" s="616"/>
+      <c r="E29" s="619"/>
       <c r="F29" s="18" t="s">
         <v>257</v>
       </c>
@@ -13036,8 +13226,8 @@
     <row r="30" spans="1:20" ht="13.15" customHeight="1">
       <c r="B30" s="278"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="599"/>
-      <c r="E30" s="602"/>
+      <c r="D30" s="616"/>
+      <c r="E30" s="619"/>
       <c r="F30" s="18" t="s">
         <v>258</v>
       </c>
@@ -13083,8 +13273,8 @@
     <row r="31" spans="1:20" ht="13.15" customHeight="1">
       <c r="B31" s="278"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="599"/>
-      <c r="E31" s="602"/>
+      <c r="D31" s="616"/>
+      <c r="E31" s="619"/>
       <c r="F31" s="18" t="s">
         <v>259</v>
       </c>
@@ -13130,8 +13320,8 @@
     <row r="32" spans="1:20" ht="13.15" customHeight="1">
       <c r="B32" s="278"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="599"/>
-      <c r="E32" s="602"/>
+      <c r="D32" s="616"/>
+      <c r="E32" s="619"/>
       <c r="F32" s="18" t="s">
         <v>260</v>
       </c>
@@ -13178,8 +13368,8 @@
     <row r="33" spans="1:20" ht="13.15" customHeight="1">
       <c r="B33" s="278"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="599"/>
-      <c r="E33" s="602"/>
+      <c r="D33" s="616"/>
+      <c r="E33" s="619"/>
       <c r="F33" s="18" t="s">
         <v>261</v>
       </c>
@@ -13225,8 +13415,8 @@
     <row r="34" spans="1:20" ht="13.15" customHeight="1">
       <c r="B34" s="278"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="599"/>
-      <c r="E34" s="602"/>
+      <c r="D34" s="616"/>
+      <c r="E34" s="619"/>
       <c r="F34" s="28" t="s">
         <v>19</v>
       </c>
@@ -13272,8 +13462,8 @@
     <row r="35" spans="1:20" ht="13.15" customHeight="1">
       <c r="B35" s="278"/>
       <c r="C35" s="33"/>
-      <c r="D35" s="599"/>
-      <c r="E35" s="603"/>
+      <c r="D35" s="616"/>
+      <c r="E35" s="620"/>
       <c r="F35" s="31" t="s">
         <v>20</v>
       </c>
@@ -13319,7 +13509,7 @@
     <row r="36" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B36" s="278"/>
       <c r="C36" s="33"/>
-      <c r="D36" s="600"/>
+      <c r="D36" s="617"/>
       <c r="E36" s="34" t="s">
         <v>125</v>
       </c>
@@ -13383,7 +13573,7 @@
     <row r="37" spans="1:20" ht="13.15" customHeight="1">
       <c r="B37" s="278"/>
       <c r="C37" s="33"/>
-      <c r="D37" s="607" t="s">
+      <c r="D37" s="603" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="58" t="s">
@@ -13433,7 +13623,7 @@
     <row r="38" spans="1:20" ht="13.15" customHeight="1">
       <c r="B38" s="278"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="608"/>
+      <c r="D38" s="604"/>
       <c r="E38" s="28" t="s">
         <v>23</v>
       </c>
@@ -13483,7 +13673,7 @@
     <row r="39" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B39" s="278"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="609"/>
+      <c r="D39" s="605"/>
       <c r="E39" s="34" t="s">
         <v>126</v>
       </c>
@@ -13571,10 +13761,10 @@
     <row r="41" spans="1:20" ht="13.15" customHeight="1">
       <c r="B41" s="278"/>
       <c r="C41" s="33"/>
-      <c r="D41" s="610" t="s">
+      <c r="D41" s="621" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="611"/>
+      <c r="E41" s="622"/>
       <c r="F41" s="31" t="s">
         <v>262</v>
       </c>
@@ -13620,8 +13810,8 @@
     <row r="42" spans="1:20" ht="13.15" customHeight="1">
       <c r="B42" s="278"/>
       <c r="C42" s="33"/>
-      <c r="D42" s="612"/>
-      <c r="E42" s="613"/>
+      <c r="D42" s="623"/>
+      <c r="E42" s="624"/>
       <c r="F42" s="31" t="s">
         <v>263</v>
       </c>
@@ -13668,10 +13858,10 @@
     <row r="43" spans="1:20" ht="13.15" customHeight="1">
       <c r="B43" s="278"/>
       <c r="C43" s="33"/>
-      <c r="D43" s="595" t="s">
+      <c r="D43" s="596" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="596"/>
+      <c r="E43" s="597"/>
       <c r="F43" s="31"/>
       <c r="G43" s="338">
         <v>29</v>
@@ -13715,10 +13905,10 @@
     <row r="44" spans="1:20" ht="13.15" customHeight="1">
       <c r="B44" s="278"/>
       <c r="C44" s="33"/>
-      <c r="D44" s="595" t="s">
+      <c r="D44" s="596" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="596"/>
+      <c r="E44" s="597"/>
       <c r="F44" s="31"/>
       <c r="G44" s="338">
         <v>30</v>
@@ -13762,10 +13952,10 @@
     <row r="45" spans="1:20" ht="13.15" customHeight="1">
       <c r="B45" s="278"/>
       <c r="C45" s="33"/>
-      <c r="D45" s="595" t="s">
+      <c r="D45" s="596" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="596"/>
+      <c r="E45" s="597"/>
       <c r="F45" s="31"/>
       <c r="G45" s="338">
         <v>31</v>
@@ -13971,7 +14161,7 @@
     <row r="50" spans="1:20">
       <c r="B50" s="278"/>
       <c r="C50" s="33"/>
-      <c r="D50" s="607" t="s">
+      <c r="D50" s="603" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="74" t="s">
@@ -14021,7 +14211,7 @@
     <row r="51" spans="1:20">
       <c r="B51" s="278"/>
       <c r="C51" s="33"/>
-      <c r="D51" s="608"/>
+      <c r="D51" s="604"/>
       <c r="E51" s="74" t="s">
         <v>36</v>
       </c>
@@ -14069,7 +14259,7 @@
     <row r="52" spans="1:20">
       <c r="B52" s="278"/>
       <c r="C52" s="33"/>
-      <c r="D52" s="608"/>
+      <c r="D52" s="604"/>
       <c r="E52" s="74" t="s">
         <v>37</v>
       </c>
@@ -14117,7 +14307,7 @@
     <row r="53" spans="1:20">
       <c r="B53" s="278"/>
       <c r="C53" s="33"/>
-      <c r="D53" s="608"/>
+      <c r="D53" s="604"/>
       <c r="E53" s="74" t="s">
         <v>38</v>
       </c>
@@ -14165,7 +14355,7 @@
     <row r="54" spans="1:20" s="37" customFormat="1" ht="13.5" thickBot="1">
       <c r="B54" s="278"/>
       <c r="C54" s="84"/>
-      <c r="D54" s="609"/>
+      <c r="D54" s="605"/>
       <c r="E54" s="170" t="s">
         <v>128</v>
       </c>
@@ -14328,7 +14518,7 @@
     <row r="58" spans="1:20">
       <c r="B58" s="278"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="623" t="s">
+      <c r="D58" s="607" t="s">
         <v>43</v>
       </c>
       <c r="E58" s="86" t="s">
@@ -14378,7 +14568,7 @@
     <row r="59" spans="1:20">
       <c r="B59" s="278"/>
       <c r="C59" s="33"/>
-      <c r="D59" s="623"/>
+      <c r="D59" s="607"/>
       <c r="E59" s="86" t="s">
         <v>45</v>
       </c>
@@ -14427,7 +14617,7 @@
       <c r="A60" s="285"/>
       <c r="B60" s="278"/>
       <c r="C60" s="33"/>
-      <c r="D60" s="623"/>
+      <c r="D60" s="607"/>
       <c r="E60" s="34" t="s">
         <v>87</v>
       </c>
@@ -14492,7 +14682,7 @@
     <row r="61" spans="1:20">
       <c r="B61" s="278"/>
       <c r="C61" s="230"/>
-      <c r="D61" s="623"/>
+      <c r="D61" s="607"/>
       <c r="E61" s="86" t="s">
         <v>104</v>
       </c>
@@ -14540,7 +14730,7 @@
     <row r="62" spans="1:20">
       <c r="B62" s="278"/>
       <c r="C62" s="33"/>
-      <c r="D62" s="623"/>
+      <c r="D62" s="607"/>
       <c r="E62" s="86" t="s">
         <v>103</v>
       </c>
@@ -14674,11 +14864,11 @@
     <row r="65" spans="1:20">
       <c r="B65" s="278"/>
       <c r="C65" s="33"/>
-      <c r="D65" s="619" t="s">
+      <c r="D65" s="595" t="s">
         <v>94</v>
       </c>
-      <c r="E65" s="619"/>
-      <c r="F65" s="619"/>
+      <c r="E65" s="595"/>
+      <c r="F65" s="595"/>
       <c r="G65" s="338">
         <v>46</v>
       </c>
@@ -14721,11 +14911,11 @@
     <row r="66" spans="1:20">
       <c r="B66" s="278"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="619" t="s">
+      <c r="D66" s="595" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="619"/>
-      <c r="F66" s="619"/>
+      <c r="E66" s="595"/>
+      <c r="F66" s="595"/>
       <c r="G66" s="338">
         <v>47</v>
       </c>
@@ -14791,11 +14981,11 @@
     <row r="68" spans="1:20">
       <c r="B68" s="278"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="619" t="s">
+      <c r="D68" s="595" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="619"/>
-      <c r="F68" s="619"/>
+      <c r="E68" s="595"/>
+      <c r="F68" s="595"/>
       <c r="G68" s="338">
         <v>48</v>
       </c>
@@ -14838,11 +15028,11 @@
     <row r="69" spans="1:20">
       <c r="B69" s="278"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="619" t="s">
+      <c r="D69" s="595" t="s">
         <v>122</v>
       </c>
-      <c r="E69" s="619"/>
-      <c r="F69" s="619"/>
+      <c r="E69" s="595"/>
+      <c r="F69" s="595"/>
       <c r="G69" s="338">
         <v>49</v>
       </c>
@@ -14885,11 +15075,11 @@
     <row r="70" spans="1:20">
       <c r="B70" s="278"/>
       <c r="C70" s="33"/>
-      <c r="D70" s="619" t="s">
+      <c r="D70" s="595" t="s">
         <v>123</v>
       </c>
-      <c r="E70" s="619"/>
-      <c r="F70" s="619"/>
+      <c r="E70" s="595"/>
+      <c r="F70" s="595"/>
       <c r="G70" s="338">
         <v>50</v>
       </c>
@@ -14955,7 +15145,7 @@
     <row r="72" spans="1:20">
       <c r="B72" s="278"/>
       <c r="C72" s="33"/>
-      <c r="D72" s="624" t="s">
+      <c r="D72" s="608" t="s">
         <v>46</v>
       </c>
       <c r="E72" s="98" t="s">
@@ -15004,7 +15194,7 @@
     <row r="73" spans="1:20">
       <c r="B73" s="278"/>
       <c r="C73" s="33"/>
-      <c r="D73" s="624"/>
+      <c r="D73" s="608"/>
       <c r="E73" s="98" t="s">
         <v>105</v>
       </c>
@@ -15052,7 +15242,7 @@
     <row r="74" spans="1:20">
       <c r="B74" s="278"/>
       <c r="C74" s="33"/>
-      <c r="D74" s="624"/>
+      <c r="D74" s="608"/>
       <c r="E74" s="98" t="s">
         <v>48</v>
       </c>
@@ -15100,7 +15290,7 @@
     <row r="75" spans="1:20">
       <c r="B75" s="278"/>
       <c r="C75" s="33"/>
-      <c r="D75" s="624"/>
+      <c r="D75" s="608"/>
       <c r="E75" s="98" t="s">
         <v>49</v>
       </c>
@@ -15148,7 +15338,7 @@
     <row r="76" spans="1:20">
       <c r="B76" s="278"/>
       <c r="C76" s="33"/>
-      <c r="D76" s="624"/>
+      <c r="D76" s="608"/>
       <c r="E76" s="98" t="s">
         <v>50</v>
       </c>
@@ -15196,7 +15386,7 @@
     <row r="77" spans="1:20">
       <c r="B77" s="278"/>
       <c r="C77" s="33"/>
-      <c r="D77" s="624"/>
+      <c r="D77" s="608"/>
       <c r="E77" s="74" t="s">
         <v>51</v>
       </c>
@@ -15375,7 +15565,7 @@
     <row r="80" spans="1:20">
       <c r="B80" s="278"/>
       <c r="C80" s="33"/>
-      <c r="D80" s="607" t="s">
+      <c r="D80" s="603" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="98" t="s">
@@ -15424,7 +15614,7 @@
     <row r="81" spans="2:20">
       <c r="B81" s="278"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="608"/>
+      <c r="D81" s="604"/>
       <c r="E81" s="98" t="s">
         <v>201</v>
       </c>
@@ -15472,7 +15662,7 @@
     <row r="82" spans="2:20">
       <c r="B82" s="278"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="608"/>
+      <c r="D82" s="604"/>
       <c r="E82" s="98" t="s">
         <v>202</v>
       </c>
@@ -15520,7 +15710,7 @@
     <row r="83" spans="2:20">
       <c r="B83" s="278"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="609"/>
+      <c r="D83" s="605"/>
       <c r="E83" s="98" t="s">
         <v>203</v>
       </c>
@@ -15633,13 +15823,13 @@
     <row r="85" spans="2:20" ht="13.15" customHeight="1">
       <c r="B85" s="278"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="622" t="s">
+      <c r="D85" s="606" t="s">
         <v>53</v>
       </c>
-      <c r="E85" s="595" t="s">
+      <c r="E85" s="596" t="s">
         <v>206</v>
       </c>
-      <c r="F85" s="596"/>
+      <c r="F85" s="597"/>
       <c r="G85" s="338">
         <f t="shared" si="10"/>
         <v>64</v>
@@ -15683,7 +15873,7 @@
     <row r="86" spans="2:20">
       <c r="B86" s="278"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="622"/>
+      <c r="D86" s="606"/>
       <c r="E86" s="98" t="s">
         <v>54</v>
       </c>
@@ -15731,7 +15921,7 @@
     <row r="87" spans="2:20">
       <c r="B87" s="278"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="622"/>
+      <c r="D87" s="606"/>
       <c r="E87" s="34" t="s">
         <v>134</v>
       </c>
@@ -15796,7 +15986,7 @@
     <row r="88" spans="2:20">
       <c r="B88" s="278"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="622" t="s">
+      <c r="D88" s="606" t="s">
         <v>55</v>
       </c>
       <c r="E88" s="98" t="s">
@@ -15846,7 +16036,7 @@
     <row r="89" spans="2:20">
       <c r="B89" s="278"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="622"/>
+      <c r="D89" s="606"/>
       <c r="E89" s="98" t="s">
         <v>56</v>
       </c>
@@ -15894,7 +16084,7 @@
     <row r="90" spans="2:20">
       <c r="B90" s="278"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="622"/>
+      <c r="D90" s="606"/>
       <c r="E90" s="98" t="s">
         <v>200</v>
       </c>
@@ -15942,7 +16132,7 @@
     <row r="91" spans="2:20">
       <c r="B91" s="278"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="607" t="s">
+      <c r="D91" s="603" t="s">
         <v>57</v>
       </c>
       <c r="E91" s="98" t="s">
@@ -15992,7 +16182,7 @@
     <row r="92" spans="2:20" s="102" customFormat="1">
       <c r="B92" s="278"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="608"/>
+      <c r="D92" s="604"/>
       <c r="E92" s="98" t="s">
         <v>58</v>
       </c>
@@ -16040,7 +16230,7 @@
     <row r="93" spans="2:20">
       <c r="B93" s="278"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="609"/>
+      <c r="D93" s="605"/>
       <c r="E93" s="98" t="s">
         <v>207</v>
       </c>
@@ -16153,11 +16343,11 @@
     <row r="95" spans="2:20">
       <c r="B95" s="278"/>
       <c r="C95" s="84"/>
-      <c r="D95" s="604" t="s">
+      <c r="D95" s="598" t="s">
         <v>59</v>
       </c>
-      <c r="E95" s="605"/>
-      <c r="F95" s="606"/>
+      <c r="E95" s="599"/>
+      <c r="F95" s="600"/>
       <c r="G95" s="338">
         <f t="shared" si="10"/>
         <v>74</v>
@@ -17540,8 +17730,8 @@
         <v>79</v>
       </c>
       <c r="D125" s="148"/>
-      <c r="E125" s="620"/>
-      <c r="F125" s="621"/>
+      <c r="E125" s="601"/>
+      <c r="F125" s="602"/>
       <c r="G125" s="338"/>
       <c r="H125" s="450"/>
       <c r="I125" s="451"/>
@@ -20023,13 +20213,15 @@
     <protectedRange sqref="H100:H104 H111:H114 H106:H107" name="Range17_1_1_1_8_1"/>
   </protectedRanges>
   <mergeCells count="28">
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="D88:D90"/>
-    <mergeCell ref="D91:D93"/>
-    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D24:D36"/>
+    <mergeCell ref="E24:E35"/>
+    <mergeCell ref="D37:D39"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:F11"/>
     <mergeCell ref="D72:D77"/>
     <mergeCell ref="D41:E42"/>
     <mergeCell ref="D43:E43"/>
@@ -20042,15 +20234,13 @@
     <mergeCell ref="D68:F68"/>
     <mergeCell ref="D69:F69"/>
     <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D24:D36"/>
-    <mergeCell ref="E24:E35"/>
-    <mergeCell ref="D37:D39"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="D91:D93"/>
+    <mergeCell ref="D95:F95"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="59" orientation="portrait" r:id="rId1"/>
@@ -20064,18 +20254,295 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629DAB4-A91A-4D1E-92A9-9AE2403D6050}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1">
+        <v>11199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2">
+        <v>5938</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B3">
+        <v>10211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B4" s="655">
+        <f>B3/B1</f>
+        <v>0.91177783730690243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="657" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>393</v>
+      </c>
+      <c r="B9">
+        <v>8731</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>395</v>
+      </c>
+      <c r="B10">
+        <v>8647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>396</v>
+      </c>
+      <c r="B11" s="655">
+        <f>B10/B9</f>
+        <v>0.99037910892223113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="656">
+        <f>B12/B1</f>
+        <v>3.8396285382623447E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="656"/>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" s="656"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="657" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>398</v>
+      </c>
+      <c r="B18" s="658">
+        <v>8.997685185185185E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>399</v>
+      </c>
+      <c r="B19" s="658">
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>402</v>
+      </c>
+      <c r="B20" s="655">
+        <f>B19/B18</f>
+        <v>1.0419346539747878</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>400</v>
+      </c>
+      <c r="B22" s="658">
+        <v>7.6006944444444446E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>401</v>
+      </c>
+      <c r="B23" s="658">
+        <v>7.2916666666666671E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>402</v>
+      </c>
+      <c r="B24" s="655">
+        <f>B23/B22</f>
+        <v>0.9593421653723162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>403</v>
+      </c>
+      <c r="B26" s="658">
+        <v>5.0405092592592592E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" s="658">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B28" s="655">
+        <f>B27/B26</f>
+        <v>0.82663605051664746</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="657" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>406</v>
+      </c>
+      <c r="B32">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>407</v>
+      </c>
+      <c r="B33" s="655">
+        <f>B32/B1</f>
+        <v>0.39494597731940351</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="657" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>409</v>
+      </c>
+      <c r="B37">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>410</v>
+      </c>
+      <c r="B38" s="656">
+        <f>B37/B2</f>
+        <v>9.2623779050185241E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="657" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>413</v>
+      </c>
+      <c r="B42">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>414</v>
+      </c>
+      <c r="B43" s="655">
+        <f>B42/B1</f>
+        <v>0.39994642378783818</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="657" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>418</v>
+      </c>
+      <c r="B47">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AE42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="B7" sqref="B7"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11:AE41"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -20690,10 +21157,10 @@
       </c>
       <c r="B4" s="505"/>
       <c r="C4" s="506"/>
-      <c r="D4" s="630" t="s">
+      <c r="D4" s="645" t="s">
         <v>334</v>
       </c>
-      <c r="E4" s="630"/>
+      <c r="E4" s="645"/>
     </row>
     <row r="5" spans="1:31" ht="26.25" customHeight="1">
       <c r="A5" s="504" t="s">
@@ -20701,10 +21168,10 @@
       </c>
       <c r="B5" s="505"/>
       <c r="C5" s="506"/>
-      <c r="D5" s="630" t="s">
+      <c r="D5" s="645" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="630"/>
+      <c r="E5" s="645"/>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="507"/>
@@ -20736,12 +21203,12 @@
       <c r="A8" s="515" t="s">
         <v>337</v>
       </c>
-      <c r="B8" s="631" t="s">
+      <c r="B8" s="646" t="s">
         <v>338</v>
       </c>
-      <c r="C8" s="632"/>
-      <c r="D8" s="632"/>
-      <c r="E8" s="633"/>
+      <c r="C8" s="647"/>
+      <c r="D8" s="647"/>
+      <c r="E8" s="648"/>
       <c r="F8" s="515"/>
       <c r="G8" s="516" t="s">
         <v>339</v>
@@ -20882,10 +21349,10 @@
     <row r="11" spans="1:31" ht="30" customHeight="1">
       <c r="A11" s="522"/>
       <c r="B11" s="510"/>
-      <c r="C11" s="634" t="s">
+      <c r="C11" s="649" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="637" t="s">
+      <c r="D11" s="652" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="532">
@@ -20973,8 +21440,8 @@
     <row r="12" spans="1:31" ht="30" customHeight="1">
       <c r="A12" s="522"/>
       <c r="B12" s="510"/>
-      <c r="C12" s="635"/>
-      <c r="D12" s="638"/>
+      <c r="C12" s="650"/>
+      <c r="D12" s="653"/>
       <c r="E12" s="532">
         <v>20</v>
       </c>
@@ -21060,8 +21527,8 @@
     <row r="13" spans="1:31" ht="30" customHeight="1">
       <c r="A13" s="522"/>
       <c r="B13" s="510"/>
-      <c r="C13" s="635"/>
-      <c r="D13" s="638"/>
+      <c r="C13" s="650"/>
+      <c r="D13" s="653"/>
       <c r="E13" s="532">
         <v>30</v>
       </c>
@@ -21147,8 +21614,8 @@
     <row r="14" spans="1:31" ht="30" customHeight="1">
       <c r="A14" s="522"/>
       <c r="B14" s="510"/>
-      <c r="C14" s="635"/>
-      <c r="D14" s="638"/>
+      <c r="C14" s="650"/>
+      <c r="D14" s="653"/>
       <c r="E14" s="532">
         <v>40</v>
       </c>
@@ -21234,8 +21701,8 @@
     <row r="15" spans="1:31" ht="30" customHeight="1">
       <c r="A15" s="522"/>
       <c r="B15" s="510"/>
-      <c r="C15" s="635"/>
-      <c r="D15" s="638"/>
+      <c r="C15" s="650"/>
+      <c r="D15" s="653"/>
       <c r="E15" s="532">
         <v>50</v>
       </c>
@@ -21321,8 +21788,8 @@
     <row r="16" spans="1:31" ht="30" customHeight="1">
       <c r="A16" s="522"/>
       <c r="B16" s="510"/>
-      <c r="C16" s="635"/>
-      <c r="D16" s="638"/>
+      <c r="C16" s="650"/>
+      <c r="D16" s="653"/>
       <c r="E16" s="532">
         <v>60</v>
       </c>
@@ -21408,8 +21875,8 @@
     <row r="17" spans="1:31" ht="30" customHeight="1">
       <c r="A17" s="522"/>
       <c r="B17" s="510"/>
-      <c r="C17" s="635"/>
-      <c r="D17" s="638"/>
+      <c r="C17" s="650"/>
+      <c r="D17" s="653"/>
       <c r="E17" s="532">
         <v>70</v>
       </c>
@@ -21495,8 +21962,8 @@
     <row r="18" spans="1:31" ht="30" customHeight="1">
       <c r="A18" s="522"/>
       <c r="B18" s="510"/>
-      <c r="C18" s="635"/>
-      <c r="D18" s="638"/>
+      <c r="C18" s="650"/>
+      <c r="D18" s="653"/>
       <c r="E18" s="532">
         <v>80</v>
       </c>
@@ -21582,8 +22049,8 @@
     <row r="19" spans="1:31" ht="30" customHeight="1">
       <c r="A19" s="522"/>
       <c r="B19" s="510"/>
-      <c r="C19" s="635"/>
-      <c r="D19" s="638"/>
+      <c r="C19" s="650"/>
+      <c r="D19" s="653"/>
       <c r="E19" s="532">
         <v>90</v>
       </c>
@@ -21669,8 +22136,8 @@
     <row r="20" spans="1:31" ht="30" customHeight="1">
       <c r="A20" s="522"/>
       <c r="B20" s="510"/>
-      <c r="C20" s="635"/>
-      <c r="D20" s="638"/>
+      <c r="C20" s="650"/>
+      <c r="D20" s="653"/>
       <c r="E20" s="532">
         <v>100</v>
       </c>
@@ -21756,8 +22223,8 @@
     <row r="21" spans="1:31" ht="30" customHeight="1">
       <c r="A21" s="522"/>
       <c r="B21" s="510"/>
-      <c r="C21" s="635"/>
-      <c r="D21" s="638"/>
+      <c r="C21" s="650"/>
+      <c r="D21" s="653"/>
       <c r="E21" s="536" t="s">
         <v>19</v>
       </c>
@@ -21793,8 +22260,8 @@
     <row r="22" spans="1:31" ht="30" customHeight="1">
       <c r="A22" s="522"/>
       <c r="B22" s="510"/>
-      <c r="C22" s="635"/>
-      <c r="D22" s="639"/>
+      <c r="C22" s="650"/>
+      <c r="D22" s="654"/>
       <c r="E22" s="539" t="s">
         <v>20</v>
       </c>
@@ -21880,7 +22347,7 @@
     <row r="23" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="541"/>
       <c r="B23" s="542"/>
-      <c r="C23" s="636"/>
+      <c r="C23" s="651"/>
       <c r="D23" s="543" t="s">
         <v>364</v>
       </c>
@@ -21969,13 +22436,13 @@
     <row r="24" spans="1:31" ht="30" customHeight="1">
       <c r="A24" s="522"/>
       <c r="B24" s="510"/>
-      <c r="C24" s="625" t="s">
+      <c r="C24" s="640" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="628" t="s">
+      <c r="D24" s="643" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="629"/>
+      <c r="E24" s="644"/>
       <c r="F24" s="526">
         <v>14</v>
       </c>
@@ -22058,7 +22525,7 @@
     <row r="25" spans="1:31" ht="30" customHeight="1">
       <c r="A25" s="522"/>
       <c r="B25" s="510"/>
-      <c r="C25" s="626"/>
+      <c r="C25" s="641"/>
       <c r="D25" s="548" t="s">
         <v>23</v>
       </c>
@@ -22147,7 +22614,7 @@
     <row r="26" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A26" s="541"/>
       <c r="B26" s="542"/>
-      <c r="C26" s="627"/>
+      <c r="C26" s="642"/>
       <c r="D26" s="543" t="s">
         <v>366</v>
       </c>
@@ -22236,10 +22703,10 @@
     <row r="27" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A27" s="541"/>
       <c r="B27" s="542"/>
-      <c r="C27" s="646" t="s">
+      <c r="C27" s="631" t="s">
         <v>368</v>
       </c>
-      <c r="D27" s="647"/>
+      <c r="D27" s="632"/>
       <c r="E27" s="549" t="s">
         <v>369</v>
       </c>
@@ -22360,10 +22827,10 @@
     <row r="29" spans="1:31" ht="30" customHeight="1">
       <c r="A29" s="522"/>
       <c r="B29" s="510"/>
-      <c r="C29" s="648" t="s">
+      <c r="C29" s="633" t="s">
         <v>371</v>
       </c>
-      <c r="D29" s="649"/>
+      <c r="D29" s="634"/>
       <c r="E29" s="539" t="s">
         <v>372</v>
       </c>
@@ -22449,8 +22916,8 @@
     <row r="30" spans="1:31" ht="30" customHeight="1">
       <c r="A30" s="522"/>
       <c r="B30" s="510"/>
-      <c r="C30" s="650"/>
-      <c r="D30" s="651"/>
+      <c r="C30" s="635"/>
+      <c r="D30" s="636"/>
       <c r="E30" s="539" t="s">
         <v>373</v>
       </c>
@@ -22536,10 +23003,10 @@
     <row r="31" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A31" s="541"/>
       <c r="B31" s="542"/>
-      <c r="C31" s="652" t="s">
+      <c r="C31" s="637" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="653"/>
+      <c r="D31" s="638"/>
       <c r="E31" s="555"/>
       <c r="F31" s="527">
         <v>20</v>
@@ -22623,10 +23090,10 @@
     <row r="32" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A32" s="541"/>
       <c r="B32" s="542"/>
-      <c r="C32" s="652" t="s">
+      <c r="C32" s="637" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="653"/>
+      <c r="D32" s="638"/>
       <c r="E32" s="555"/>
       <c r="F32" s="527">
         <v>21</v>
@@ -22660,10 +23127,10 @@
     <row r="33" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A33" s="541"/>
       <c r="B33" s="542"/>
-      <c r="C33" s="652" t="s">
+      <c r="C33" s="637" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="653"/>
+      <c r="D33" s="638"/>
       <c r="E33" s="555"/>
       <c r="F33" s="527">
         <v>22</v>
@@ -22697,10 +23164,10 @@
     <row r="34" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A34" s="541"/>
       <c r="B34" s="558"/>
-      <c r="C34" s="646" t="s">
+      <c r="C34" s="631" t="s">
         <v>374</v>
       </c>
-      <c r="D34" s="654"/>
+      <c r="D34" s="639"/>
       <c r="E34" s="549" t="s">
         <v>375</v>
       </c>
@@ -22735,11 +23202,11 @@
     </row>
     <row r="35" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A35" s="559"/>
-      <c r="B35" s="640" t="s">
+      <c r="B35" s="625" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="641"/>
-      <c r="D35" s="642"/>
+      <c r="C35" s="626"/>
+      <c r="D35" s="627"/>
       <c r="E35" s="560" t="s">
         <v>377</v>
       </c>
@@ -22862,7 +23329,7 @@
     <row r="37" spans="1:31" ht="30" customHeight="1">
       <c r="A37" s="563"/>
       <c r="B37" s="571"/>
-      <c r="C37" s="643" t="s">
+      <c r="C37" s="628" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="572" t="s">
@@ -22951,7 +23418,7 @@
     <row r="38" spans="1:31" ht="30" customHeight="1">
       <c r="A38" s="563"/>
       <c r="B38" s="571"/>
-      <c r="C38" s="644"/>
+      <c r="C38" s="629"/>
       <c r="D38" s="572" t="s">
         <v>36</v>
       </c>
@@ -23038,7 +23505,7 @@
     <row r="39" spans="1:31" ht="30" customHeight="1">
       <c r="A39" s="563"/>
       <c r="B39" s="571"/>
-      <c r="C39" s="644"/>
+      <c r="C39" s="629"/>
       <c r="D39" s="572" t="s">
         <v>37</v>
       </c>
@@ -23125,7 +23592,7 @@
     <row r="40" spans="1:31" ht="30" customHeight="1">
       <c r="A40" s="563"/>
       <c r="B40" s="571"/>
-      <c r="C40" s="644"/>
+      <c r="C40" s="629"/>
       <c r="D40" s="572" t="s">
         <v>38</v>
       </c>
@@ -23162,7 +23629,7 @@
     <row r="41" spans="1:31" ht="30" customHeight="1" thickBot="1">
       <c r="A41" s="576"/>
       <c r="B41" s="577"/>
-      <c r="C41" s="645"/>
+      <c r="C41" s="630"/>
       <c r="D41" s="578" t="s">
         <v>379</v>
       </c>
@@ -23282,6 +23749,13 @@
     <protectedRange sqref="N12:N22 N28:N33" name="Range16_1_1_1_6_3_1"/>
   </protectedRanges>
   <mergeCells count="15">
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="C11:C23"/>
+    <mergeCell ref="D11:D22"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="C37:C41"/>
     <mergeCell ref="C27:D27"/>
@@ -23290,13 +23764,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="C11:C23"/>
-    <mergeCell ref="D11:D22"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Membuat pareto pada Problem Analisys
</commit_message>
<xml_diff>
--- a/Data-Data/Laporan KPI GR 2020 Auto2000 Banyuwangi.xlsx
+++ b/Data-Data/Laporan KPI GR 2020 Auto2000 Banyuwangi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT_WIndows\Kaizen2021\Data-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AB47A-9BCD-4FD6-9A15-773DAC109DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356E4366-57BF-440F-814E-D4AC8E214213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Guidance!$B$1:$U$177</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'KPI A2000 Banyuwangi'!$B$1:$T$148</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="431">
   <si>
     <t>BRANCH_NAME</t>
   </si>
@@ -1838,6 +1838,36 @@
   </si>
   <si>
     <t>SBI Same Outlet (%)</t>
+  </si>
+  <si>
+    <t>DTR</t>
+  </si>
+  <si>
+    <t>Qwantity</t>
+  </si>
+  <si>
+    <t>Qwality</t>
+  </si>
+  <si>
+    <t>CPS</t>
+  </si>
+  <si>
+    <t>Revenue Part(x 1000)</t>
+  </si>
+  <si>
+    <t>Comsumption Part per Service</t>
+  </si>
+  <si>
+    <t>EM Contribution</t>
+  </si>
+  <si>
+    <t>Ach</t>
+  </si>
+  <si>
+    <t>App Rate</t>
+  </si>
+  <si>
+    <t>TMO Share</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2983,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="659">
+  <cellXfs count="661">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -4901,191 +4931,193 @@
     </xf>
     <xf numFmtId="170" fontId="2" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="41" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="42" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="43" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="25" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="26" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="30" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="31" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="11" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="24" fillId="0" borderId="12" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="41" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="42" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="43" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="25" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="26" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="30" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="31" xfId="24" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="11" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="12" xfId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="24" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="4" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="AutoFormat-Optionen" xfId="18" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -5127,6 +5159,1296 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ID"/>
+              <a:t>Pareto</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-ID" baseline="0"/>
+              <a:t> Problem</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-ID"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000008-604F-4338-9BD6-69842CC54299}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-604F-4338-9BD6-69842CC54299}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-604F-4338-9BD6-69842CC54299}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-604F-4338-9BD6-69842CC54299}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FF0000"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-604F-4338-9BD6-69842CC54299}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="0070C0"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$11:$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>EM Contribution</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>App Rate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Leadtime EM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TMO Share</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Leadtime SBE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$11:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.8139534883720929E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20348837209302326</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.24127906976744184</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.27034883720930236</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27906976744186046</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-604F-4338-9BD6-69842CC54299}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="472186960"/>
+        <c:axId val="472181712"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$11:$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>EM Contribution</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>App Rate</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Leadtime EM</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TMO Share</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Leadtime SBE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$11:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21348837209302327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.45476744186046514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7251162790697675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0041860465116279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-604F-4338-9BD6-69842CC54299}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="462257256"/>
+        <c:axId val="468765160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="472186960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472181712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="472181712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="472186960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="468765160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="462257256"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="462257256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="468765160"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5580,6 +6902,47 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806D139F-2C16-4B93-848A-40795A4516CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6308,8 +7671,8 @@
       </c>
       <c r="C3" s="100"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="609"/>
-      <c r="F3" s="609"/>
+      <c r="E3" s="613"/>
+      <c r="F3" s="613"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -6327,8 +7690,8 @@
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="31"/>
-      <c r="E4" s="609"/>
-      <c r="F4" s="609"/>
+      <c r="E4" s="613"/>
+      <c r="F4" s="613"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -6365,12 +7728,12 @@
       <c r="B6" s="206" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="610" t="s">
+      <c r="C6" s="614" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="611"/>
-      <c r="E6" s="611"/>
-      <c r="F6" s="612"/>
+      <c r="D6" s="615"/>
+      <c r="E6" s="615"/>
+      <c r="F6" s="616"/>
       <c r="G6" s="206"/>
       <c r="H6" s="224" t="s">
         <v>137</v>
@@ -6441,11 +7804,11 @@
     <row r="8" spans="1:21" s="37" customFormat="1">
       <c r="B8" s="278"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="598" t="s">
+      <c r="D8" s="602" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="599"/>
-      <c r="F8" s="600"/>
+      <c r="E8" s="603"/>
+      <c r="F8" s="604"/>
       <c r="G8" s="49"/>
       <c r="H8" s="177"/>
       <c r="I8" s="177"/>
@@ -6488,7 +7851,7 @@
       <c r="R9" s="56"/>
       <c r="S9" s="56"/>
       <c r="T9" s="43"/>
-      <c r="U9" s="614" t="s">
+      <c r="U9" s="618" t="s">
         <v>227</v>
       </c>
     </row>
@@ -6518,16 +7881,16 @@
       <c r="R10" s="56"/>
       <c r="S10" s="56"/>
       <c r="T10" s="43"/>
-      <c r="U10" s="614"/>
+      <c r="U10" s="618"/>
     </row>
     <row r="11" spans="1:21" s="37" customFormat="1">
       <c r="B11" s="278"/>
       <c r="C11" s="33"/>
-      <c r="D11" s="598" t="s">
+      <c r="D11" s="602" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="599"/>
-      <c r="F11" s="600"/>
+      <c r="E11" s="603"/>
+      <c r="F11" s="604"/>
       <c r="G11" s="51"/>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
@@ -6570,7 +7933,7 @@
       <c r="R12" s="56"/>
       <c r="S12" s="56"/>
       <c r="T12" s="43"/>
-      <c r="U12" s="614" t="s">
+      <c r="U12" s="618" t="s">
         <v>228</v>
       </c>
     </row>
@@ -6600,7 +7963,7 @@
       <c r="R13" s="56"/>
       <c r="S13" s="56"/>
       <c r="T13" s="43"/>
-      <c r="U13" s="614"/>
+      <c r="U13" s="618"/>
     </row>
     <row r="14" spans="1:21" s="37" customFormat="1">
       <c r="B14" s="278"/>
@@ -6652,7 +8015,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
       <c r="T15" s="245"/>
-      <c r="U15" s="614" t="s">
+      <c r="U15" s="618" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6682,7 +8045,7 @@
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
       <c r="T16" s="245"/>
-      <c r="U16" s="614"/>
+      <c r="U16" s="618"/>
     </row>
     <row r="17" spans="1:23" s="47" customFormat="1">
       <c r="A17" s="37"/>
@@ -6743,10 +8106,10 @@
     <row r="19" spans="1:23" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B19" s="278"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="598" t="s">
+      <c r="D19" s="602" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="613"/>
+      <c r="E19" s="617"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="H19" s="177"/>
@@ -6920,10 +8283,10 @@
     <row r="24" spans="1:23" ht="13.15" customHeight="1">
       <c r="B24" s="278"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="615" t="s">
+      <c r="D24" s="619" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="618" t="s">
+      <c r="E24" s="622" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
@@ -6952,8 +8315,8 @@
     <row r="25" spans="1:23" ht="13.15" customHeight="1">
       <c r="B25" s="278"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="616"/>
-      <c r="E25" s="619"/>
+      <c r="D25" s="620"/>
+      <c r="E25" s="623"/>
       <c r="F25" s="18" t="s">
         <v>253</v>
       </c>
@@ -6980,8 +8343,8 @@
     <row r="26" spans="1:23">
       <c r="B26" s="278"/>
       <c r="C26" s="33"/>
-      <c r="D26" s="616"/>
-      <c r="E26" s="619"/>
+      <c r="D26" s="620"/>
+      <c r="E26" s="623"/>
       <c r="F26" s="18" t="s">
         <v>254</v>
       </c>
@@ -7009,8 +8372,8 @@
     <row r="27" spans="1:23" ht="13.15" customHeight="1">
       <c r="B27" s="278"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="616"/>
-      <c r="E27" s="619"/>
+      <c r="D27" s="620"/>
+      <c r="E27" s="623"/>
       <c r="F27" s="18" t="s">
         <v>255</v>
       </c>
@@ -7037,8 +8400,8 @@
     <row r="28" spans="1:23" ht="13.15" customHeight="1">
       <c r="B28" s="278"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="616"/>
-      <c r="E28" s="619"/>
+      <c r="D28" s="620"/>
+      <c r="E28" s="623"/>
       <c r="F28" s="18" t="s">
         <v>256</v>
       </c>
@@ -7067,8 +8430,8 @@
     <row r="29" spans="1:23" ht="13.15" customHeight="1">
       <c r="B29" s="278"/>
       <c r="C29" s="33"/>
-      <c r="D29" s="616"/>
-      <c r="E29" s="619"/>
+      <c r="D29" s="620"/>
+      <c r="E29" s="623"/>
       <c r="F29" s="18" t="s">
         <v>257</v>
       </c>
@@ -7097,8 +8460,8 @@
     <row r="30" spans="1:23" ht="13.15" customHeight="1">
       <c r="B30" s="278"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="616"/>
-      <c r="E30" s="619"/>
+      <c r="D30" s="620"/>
+      <c r="E30" s="623"/>
       <c r="F30" s="18" t="s">
         <v>258</v>
       </c>
@@ -7127,8 +8490,8 @@
     <row r="31" spans="1:23" ht="13.15" customHeight="1">
       <c r="B31" s="278"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="616"/>
-      <c r="E31" s="619"/>
+      <c r="D31" s="620"/>
+      <c r="E31" s="623"/>
       <c r="F31" s="18" t="s">
         <v>259</v>
       </c>
@@ -7157,8 +8520,8 @@
     <row r="32" spans="1:23" ht="13.15" customHeight="1">
       <c r="B32" s="278"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="616"/>
-      <c r="E32" s="619"/>
+      <c r="D32" s="620"/>
+      <c r="E32" s="623"/>
       <c r="F32" s="18" t="s">
         <v>260</v>
       </c>
@@ -7188,8 +8551,8 @@
     <row r="33" spans="1:21" ht="13.15" customHeight="1">
       <c r="B33" s="278"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="616"/>
-      <c r="E33" s="619"/>
+      <c r="D33" s="620"/>
+      <c r="E33" s="623"/>
       <c r="F33" s="18" t="s">
         <v>261</v>
       </c>
@@ -7215,8 +8578,8 @@
     <row r="34" spans="1:21" ht="13.15" customHeight="1">
       <c r="B34" s="278"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="616"/>
-      <c r="E34" s="619"/>
+      <c r="D34" s="620"/>
+      <c r="E34" s="623"/>
       <c r="F34" s="28" t="s">
         <v>19</v>
       </c>
@@ -7245,8 +8608,8 @@
     <row r="35" spans="1:21" ht="13.15" customHeight="1">
       <c r="B35" s="278"/>
       <c r="C35" s="33"/>
-      <c r="D35" s="616"/>
-      <c r="E35" s="620"/>
+      <c r="D35" s="620"/>
+      <c r="E35" s="624"/>
       <c r="F35" s="31" t="s">
         <v>20</v>
       </c>
@@ -7273,7 +8636,7 @@
     <row r="36" spans="1:21" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B36" s="278"/>
       <c r="C36" s="33"/>
-      <c r="D36" s="617"/>
+      <c r="D36" s="621"/>
       <c r="E36" s="34" t="s">
         <v>125</v>
       </c>
@@ -7338,7 +8701,7 @@
     <row r="37" spans="1:21" ht="13.15" customHeight="1">
       <c r="B37" s="278"/>
       <c r="C37" s="33"/>
-      <c r="D37" s="603" t="s">
+      <c r="D37" s="607" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="58" t="s">
@@ -7369,7 +8732,7 @@
     <row r="38" spans="1:21" ht="13.15" customHeight="1">
       <c r="B38" s="278"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="604"/>
+      <c r="D38" s="608"/>
       <c r="E38" s="28" t="s">
         <v>23</v>
       </c>
@@ -7400,7 +8763,7 @@
     <row r="39" spans="1:21" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B39" s="278"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="605"/>
+      <c r="D39" s="609"/>
       <c r="E39" s="34" t="s">
         <v>126</v>
       </c>
@@ -7490,10 +8853,10 @@
     <row r="41" spans="1:21" ht="13.15" customHeight="1">
       <c r="B41" s="278"/>
       <c r="C41" s="33"/>
-      <c r="D41" s="621" t="s">
+      <c r="D41" s="625" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="622"/>
+      <c r="E41" s="626"/>
       <c r="F41" s="31" t="s">
         <v>262</v>
       </c>
@@ -7520,8 +8883,8 @@
     <row r="42" spans="1:21" ht="13.15" customHeight="1">
       <c r="B42" s="278"/>
       <c r="C42" s="33"/>
-      <c r="D42" s="623"/>
-      <c r="E42" s="624"/>
+      <c r="D42" s="627"/>
+      <c r="E42" s="628"/>
       <c r="F42" s="31" t="s">
         <v>263</v>
       </c>
@@ -7551,10 +8914,10 @@
     <row r="43" spans="1:21" ht="13.15" customHeight="1">
       <c r="B43" s="278"/>
       <c r="C43" s="33"/>
-      <c r="D43" s="596" t="s">
+      <c r="D43" s="600" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="597"/>
+      <c r="E43" s="601"/>
       <c r="F43" s="31"/>
       <c r="G43" s="274">
         <v>29</v>
@@ -7579,10 +8942,10 @@
     <row r="44" spans="1:21" ht="13.15" customHeight="1">
       <c r="B44" s="278"/>
       <c r="C44" s="33"/>
-      <c r="D44" s="596" t="s">
+      <c r="D44" s="600" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="597"/>
+      <c r="E44" s="601"/>
       <c r="F44" s="31"/>
       <c r="G44" s="274">
         <v>30</v>
@@ -7607,10 +8970,10 @@
     <row r="45" spans="1:21" ht="13.15" customHeight="1">
       <c r="B45" s="278"/>
       <c r="C45" s="33"/>
-      <c r="D45" s="596" t="s">
+      <c r="D45" s="600" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="597"/>
+      <c r="E45" s="601"/>
       <c r="F45" s="31"/>
       <c r="G45" s="274">
         <v>31</v>
@@ -7783,7 +9146,7 @@
     <row r="50" spans="1:21">
       <c r="B50" s="278"/>
       <c r="C50" s="33"/>
-      <c r="D50" s="603" t="s">
+      <c r="D50" s="607" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="74" t="s">
@@ -7816,7 +9179,7 @@
     <row r="51" spans="1:21">
       <c r="B51" s="278"/>
       <c r="C51" s="33"/>
-      <c r="D51" s="604"/>
+      <c r="D51" s="608"/>
       <c r="E51" s="74" t="s">
         <v>36</v>
       </c>
@@ -7847,7 +9210,7 @@
     <row r="52" spans="1:21">
       <c r="B52" s="278"/>
       <c r="C52" s="33"/>
-      <c r="D52" s="604"/>
+      <c r="D52" s="608"/>
       <c r="E52" s="74" t="s">
         <v>37</v>
       </c>
@@ -7878,7 +9241,7 @@
     <row r="53" spans="1:21">
       <c r="B53" s="278"/>
       <c r="C53" s="33"/>
-      <c r="D53" s="604"/>
+      <c r="D53" s="608"/>
       <c r="E53" s="74" t="s">
         <v>38</v>
       </c>
@@ -7909,7 +9272,7 @@
     <row r="54" spans="1:21" s="37" customFormat="1" ht="13.5" thickBot="1">
       <c r="B54" s="278"/>
       <c r="C54" s="84"/>
-      <c r="D54" s="605"/>
+      <c r="D54" s="609"/>
       <c r="E54" s="170" t="s">
         <v>128</v>
       </c>
@@ -8060,7 +9423,7 @@
     <row r="58" spans="1:21">
       <c r="B58" s="278"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="607" t="s">
+      <c r="D58" s="611" t="s">
         <v>43</v>
       </c>
       <c r="E58" s="86" t="s">
@@ -8093,7 +9456,7 @@
     <row r="59" spans="1:21">
       <c r="B59" s="278"/>
       <c r="C59" s="33"/>
-      <c r="D59" s="607"/>
+      <c r="D59" s="611"/>
       <c r="E59" s="86" t="s">
         <v>45</v>
       </c>
@@ -8125,7 +9488,7 @@
       <c r="A60" s="285"/>
       <c r="B60" s="278"/>
       <c r="C60" s="33"/>
-      <c r="D60" s="607"/>
+      <c r="D60" s="611"/>
       <c r="E60" s="34" t="s">
         <v>87</v>
       </c>
@@ -8193,7 +9556,7 @@
     <row r="61" spans="1:21">
       <c r="B61" s="278"/>
       <c r="C61" s="230"/>
-      <c r="D61" s="607"/>
+      <c r="D61" s="611"/>
       <c r="E61" s="86" t="s">
         <v>104</v>
       </c>
@@ -8224,7 +9587,7 @@
     <row r="62" spans="1:21">
       <c r="B62" s="278"/>
       <c r="C62" s="33"/>
-      <c r="D62" s="607"/>
+      <c r="D62" s="611"/>
       <c r="E62" s="86" t="s">
         <v>103</v>
       </c>
@@ -8345,11 +9708,11 @@
     <row r="65" spans="1:21">
       <c r="B65" s="278"/>
       <c r="C65" s="33"/>
-      <c r="D65" s="595" t="s">
+      <c r="D65" s="599" t="s">
         <v>94</v>
       </c>
-      <c r="E65" s="595"/>
-      <c r="F65" s="595"/>
+      <c r="E65" s="599"/>
+      <c r="F65" s="599"/>
       <c r="G65" s="274">
         <v>46</v>
       </c>
@@ -8375,11 +9738,11 @@
     <row r="66" spans="1:21">
       <c r="B66" s="278"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="595" t="s">
+      <c r="D66" s="599" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="595"/>
-      <c r="F66" s="595"/>
+      <c r="E66" s="599"/>
+      <c r="F66" s="599"/>
       <c r="G66" s="274">
         <v>47</v>
       </c>
@@ -8429,11 +9792,11 @@
     <row r="68" spans="1:21">
       <c r="B68" s="278"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="595" t="s">
+      <c r="D68" s="599" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="595"/>
-      <c r="F68" s="595"/>
+      <c r="E68" s="599"/>
+      <c r="F68" s="599"/>
       <c r="G68" s="274">
         <v>48</v>
       </c>
@@ -8459,11 +9822,11 @@
     <row r="69" spans="1:21">
       <c r="B69" s="278"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="595" t="s">
+      <c r="D69" s="599" t="s">
         <v>122</v>
       </c>
-      <c r="E69" s="595"/>
-      <c r="F69" s="595"/>
+      <c r="E69" s="599"/>
+      <c r="F69" s="599"/>
       <c r="G69" s="274">
         <v>49</v>
       </c>
@@ -8489,11 +9852,11 @@
     <row r="70" spans="1:21">
       <c r="B70" s="278"/>
       <c r="C70" s="33"/>
-      <c r="D70" s="595" t="s">
+      <c r="D70" s="599" t="s">
         <v>123</v>
       </c>
-      <c r="E70" s="595"/>
-      <c r="F70" s="595"/>
+      <c r="E70" s="599"/>
+      <c r="F70" s="599"/>
       <c r="G70" s="274">
         <v>50</v>
       </c>
@@ -8543,7 +9906,7 @@
     <row r="72" spans="1:21">
       <c r="B72" s="278"/>
       <c r="C72" s="33"/>
-      <c r="D72" s="608" t="s">
+      <c r="D72" s="612" t="s">
         <v>46</v>
       </c>
       <c r="E72" s="98" t="s">
@@ -8575,7 +9938,7 @@
     <row r="73" spans="1:21">
       <c r="B73" s="278"/>
       <c r="C73" s="33"/>
-      <c r="D73" s="608"/>
+      <c r="D73" s="612"/>
       <c r="E73" s="98" t="s">
         <v>105</v>
       </c>
@@ -8606,7 +9969,7 @@
     <row r="74" spans="1:21">
       <c r="B74" s="278"/>
       <c r="C74" s="33"/>
-      <c r="D74" s="608"/>
+      <c r="D74" s="612"/>
       <c r="E74" s="98" t="s">
         <v>48</v>
       </c>
@@ -8637,7 +10000,7 @@
     <row r="75" spans="1:21">
       <c r="B75" s="278"/>
       <c r="C75" s="33"/>
-      <c r="D75" s="608"/>
+      <c r="D75" s="612"/>
       <c r="E75" s="98" t="s">
         <v>49</v>
       </c>
@@ -8668,7 +10031,7 @@
     <row r="76" spans="1:21">
       <c r="B76" s="278"/>
       <c r="C76" s="33"/>
-      <c r="D76" s="608"/>
+      <c r="D76" s="612"/>
       <c r="E76" s="98" t="s">
         <v>50</v>
       </c>
@@ -8699,7 +10062,7 @@
     <row r="77" spans="1:21">
       <c r="B77" s="278"/>
       <c r="C77" s="33"/>
-      <c r="D77" s="608"/>
+      <c r="D77" s="612"/>
       <c r="E77" s="74" t="s">
         <v>51</v>
       </c>
@@ -8867,7 +10230,7 @@
     <row r="80" spans="1:21">
       <c r="B80" s="278"/>
       <c r="C80" s="33"/>
-      <c r="D80" s="603" t="s">
+      <c r="D80" s="607" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="98" t="s">
@@ -8899,7 +10262,7 @@
     <row r="81" spans="2:21">
       <c r="B81" s="278"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="604"/>
+      <c r="D81" s="608"/>
       <c r="E81" s="98" t="s">
         <v>201</v>
       </c>
@@ -8930,7 +10293,7 @@
     <row r="82" spans="2:21">
       <c r="B82" s="278"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="604"/>
+      <c r="D82" s="608"/>
       <c r="E82" s="98" t="s">
         <v>202</v>
       </c>
@@ -8961,7 +10324,7 @@
     <row r="83" spans="2:21">
       <c r="B83" s="278"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="605"/>
+      <c r="D83" s="609"/>
       <c r="E83" s="98" t="s">
         <v>203</v>
       </c>
@@ -9060,13 +10423,13 @@
     <row r="85" spans="2:21" ht="13.15" customHeight="1">
       <c r="B85" s="278"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="606" t="s">
+      <c r="D85" s="610" t="s">
         <v>53</v>
       </c>
-      <c r="E85" s="596" t="s">
+      <c r="E85" s="600" t="s">
         <v>206</v>
       </c>
-      <c r="F85" s="597"/>
+      <c r="F85" s="601"/>
       <c r="G85" s="274">
         <f t="shared" si="11"/>
         <v>64</v>
@@ -9093,7 +10456,7 @@
     <row r="86" spans="2:21">
       <c r="B86" s="278"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="606"/>
+      <c r="D86" s="610"/>
       <c r="E86" s="98" t="s">
         <v>54</v>
       </c>
@@ -9124,7 +10487,7 @@
     <row r="87" spans="2:21">
       <c r="B87" s="278"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="606"/>
+      <c r="D87" s="610"/>
       <c r="E87" s="34" t="s">
         <v>134</v>
       </c>
@@ -9192,7 +10555,7 @@
     <row r="88" spans="2:21">
       <c r="B88" s="278"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="606" t="s">
+      <c r="D88" s="610" t="s">
         <v>55</v>
       </c>
       <c r="E88" s="98" t="s">
@@ -9225,7 +10588,7 @@
     <row r="89" spans="2:21">
       <c r="B89" s="278"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="606"/>
+      <c r="D89" s="610"/>
       <c r="E89" s="98" t="s">
         <v>56</v>
       </c>
@@ -9256,7 +10619,7 @@
     <row r="90" spans="2:21">
       <c r="B90" s="278"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="606"/>
+      <c r="D90" s="610"/>
       <c r="E90" s="98" t="s">
         <v>200</v>
       </c>
@@ -9287,7 +10650,7 @@
     <row r="91" spans="2:21">
       <c r="B91" s="278"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="603" t="s">
+      <c r="D91" s="607" t="s">
         <v>57</v>
       </c>
       <c r="E91" s="98" t="s">
@@ -9320,7 +10683,7 @@
     <row r="92" spans="2:21" s="102" customFormat="1">
       <c r="B92" s="278"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="604"/>
+      <c r="D92" s="608"/>
       <c r="E92" s="98" t="s">
         <v>58</v>
       </c>
@@ -9351,7 +10714,7 @@
     <row r="93" spans="2:21">
       <c r="B93" s="278"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="605"/>
+      <c r="D93" s="609"/>
       <c r="E93" s="98" t="s">
         <v>207</v>
       </c>
@@ -9450,11 +10813,11 @@
     <row r="95" spans="2:21">
       <c r="B95" s="278"/>
       <c r="C95" s="84"/>
-      <c r="D95" s="598" t="s">
+      <c r="D95" s="602" t="s">
         <v>59</v>
       </c>
-      <c r="E95" s="599"/>
-      <c r="F95" s="600"/>
+      <c r="E95" s="603"/>
+      <c r="F95" s="604"/>
       <c r="G95" s="274">
         <f t="shared" si="11"/>
         <v>74</v>
@@ -10498,8 +11861,8 @@
         <v>79</v>
       </c>
       <c r="D125" s="148"/>
-      <c r="E125" s="601"/>
-      <c r="F125" s="602"/>
+      <c r="E125" s="605"/>
+      <c r="F125" s="606"/>
       <c r="G125" s="274"/>
       <c r="H125" s="226"/>
       <c r="I125" s="147"/>
@@ -12132,9 +13495,9 @@
   <dimension ref="A1:T179"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C4" sqref="C4"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41:R41"/>
+      <selection pane="bottomLeft" activeCell="F145" sqref="F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -12185,8 +13548,8 @@
       </c>
       <c r="C3" s="100"/>
       <c r="D3" s="31"/>
-      <c r="E3" s="609"/>
-      <c r="F3" s="609"/>
+      <c r="E3" s="613"/>
+      <c r="F3" s="613"/>
       <c r="H3" s="182"/>
       <c r="I3" s="182"/>
       <c r="J3" s="182"/>
@@ -12200,8 +13563,8 @@
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="31"/>
-      <c r="E4" s="609"/>
-      <c r="F4" s="609"/>
+      <c r="E4" s="613"/>
+      <c r="F4" s="613"/>
       <c r="H4" s="355"/>
       <c r="I4" s="355"/>
       <c r="J4" s="355"/>
@@ -12237,12 +13600,12 @@
       <c r="B6" s="206" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="610" t="s">
+      <c r="C6" s="614" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="611"/>
-      <c r="E6" s="611"/>
-      <c r="F6" s="612"/>
+      <c r="D6" s="615"/>
+      <c r="E6" s="615"/>
+      <c r="F6" s="616"/>
       <c r="G6" s="206"/>
       <c r="H6" s="224" t="s">
         <v>137</v>
@@ -12312,11 +13675,11 @@
     <row r="8" spans="1:20" s="37" customFormat="1">
       <c r="B8" s="278"/>
       <c r="C8" s="33"/>
-      <c r="D8" s="598" t="s">
+      <c r="D8" s="602" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="599"/>
-      <c r="F8" s="600"/>
+      <c r="E8" s="603"/>
+      <c r="F8" s="604"/>
       <c r="G8" s="49"/>
       <c r="H8" s="361"/>
       <c r="I8" s="361"/>
@@ -12429,11 +13792,11 @@
     <row r="11" spans="1:20" s="37" customFormat="1">
       <c r="B11" s="278"/>
       <c r="C11" s="33"/>
-      <c r="D11" s="598" t="s">
+      <c r="D11" s="602" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="599"/>
-      <c r="F11" s="600"/>
+      <c r="E11" s="603"/>
+      <c r="F11" s="604"/>
       <c r="G11" s="51"/>
       <c r="H11" s="366"/>
       <c r="I11" s="366"/>
@@ -12735,10 +14098,10 @@
     <row r="19" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B19" s="278"/>
       <c r="C19" s="33"/>
-      <c r="D19" s="598" t="s">
+      <c r="D19" s="602" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="613"/>
+      <c r="E19" s="617"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
       <c r="H19" s="361"/>
@@ -12939,10 +14302,10 @@
     <row r="24" spans="1:20" ht="13.15" customHeight="1">
       <c r="B24" s="278"/>
       <c r="C24" s="33"/>
-      <c r="D24" s="615" t="s">
+      <c r="D24" s="619" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="618" t="s">
+      <c r="E24" s="622" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
@@ -12990,8 +14353,8 @@
     <row r="25" spans="1:20" ht="13.15" customHeight="1">
       <c r="B25" s="278"/>
       <c r="C25" s="33"/>
-      <c r="D25" s="616"/>
-      <c r="E25" s="619"/>
+      <c r="D25" s="620"/>
+      <c r="E25" s="623"/>
       <c r="F25" s="18" t="s">
         <v>253</v>
       </c>
@@ -13037,8 +14400,8 @@
     <row r="26" spans="1:20">
       <c r="B26" s="278"/>
       <c r="C26" s="33"/>
-      <c r="D26" s="616"/>
-      <c r="E26" s="619"/>
+      <c r="D26" s="620"/>
+      <c r="E26" s="623"/>
       <c r="F26" s="18" t="s">
         <v>254</v>
       </c>
@@ -13085,8 +14448,8 @@
     <row r="27" spans="1:20" ht="13.15" customHeight="1">
       <c r="B27" s="278"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="616"/>
-      <c r="E27" s="619"/>
+      <c r="D27" s="620"/>
+      <c r="E27" s="623"/>
       <c r="F27" s="18" t="s">
         <v>255</v>
       </c>
@@ -13132,8 +14495,8 @@
     <row r="28" spans="1:20" ht="13.15" customHeight="1">
       <c r="B28" s="278"/>
       <c r="C28" s="33"/>
-      <c r="D28" s="616"/>
-      <c r="E28" s="619"/>
+      <c r="D28" s="620"/>
+      <c r="E28" s="623"/>
       <c r="F28" s="18" t="s">
         <v>256</v>
       </c>
@@ -13179,8 +14542,8 @@
     <row r="29" spans="1:20" ht="13.15" customHeight="1">
       <c r="B29" s="278"/>
       <c r="C29" s="33"/>
-      <c r="D29" s="616"/>
-      <c r="E29" s="619"/>
+      <c r="D29" s="620"/>
+      <c r="E29" s="623"/>
       <c r="F29" s="18" t="s">
         <v>257</v>
       </c>
@@ -13226,8 +14589,8 @@
     <row r="30" spans="1:20" ht="13.15" customHeight="1">
       <c r="B30" s="278"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="616"/>
-      <c r="E30" s="619"/>
+      <c r="D30" s="620"/>
+      <c r="E30" s="623"/>
       <c r="F30" s="18" t="s">
         <v>258</v>
       </c>
@@ -13273,8 +14636,8 @@
     <row r="31" spans="1:20" ht="13.15" customHeight="1">
       <c r="B31" s="278"/>
       <c r="C31" s="33"/>
-      <c r="D31" s="616"/>
-      <c r="E31" s="619"/>
+      <c r="D31" s="620"/>
+      <c r="E31" s="623"/>
       <c r="F31" s="18" t="s">
         <v>259</v>
       </c>
@@ -13320,8 +14683,8 @@
     <row r="32" spans="1:20" ht="13.15" customHeight="1">
       <c r="B32" s="278"/>
       <c r="C32" s="33"/>
-      <c r="D32" s="616"/>
-      <c r="E32" s="619"/>
+      <c r="D32" s="620"/>
+      <c r="E32" s="623"/>
       <c r="F32" s="18" t="s">
         <v>260</v>
       </c>
@@ -13368,8 +14731,8 @@
     <row r="33" spans="1:20" ht="13.15" customHeight="1">
       <c r="B33" s="278"/>
       <c r="C33" s="33"/>
-      <c r="D33" s="616"/>
-      <c r="E33" s="619"/>
+      <c r="D33" s="620"/>
+      <c r="E33" s="623"/>
       <c r="F33" s="18" t="s">
         <v>261</v>
       </c>
@@ -13415,8 +14778,8 @@
     <row r="34" spans="1:20" ht="13.15" customHeight="1">
       <c r="B34" s="278"/>
       <c r="C34" s="33"/>
-      <c r="D34" s="616"/>
-      <c r="E34" s="619"/>
+      <c r="D34" s="620"/>
+      <c r="E34" s="623"/>
       <c r="F34" s="28" t="s">
         <v>19</v>
       </c>
@@ -13462,8 +14825,8 @@
     <row r="35" spans="1:20" ht="13.15" customHeight="1">
       <c r="B35" s="278"/>
       <c r="C35" s="33"/>
-      <c r="D35" s="616"/>
-      <c r="E35" s="620"/>
+      <c r="D35" s="620"/>
+      <c r="E35" s="624"/>
       <c r="F35" s="31" t="s">
         <v>20</v>
       </c>
@@ -13509,7 +14872,7 @@
     <row r="36" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B36" s="278"/>
       <c r="C36" s="33"/>
-      <c r="D36" s="617"/>
+      <c r="D36" s="621"/>
       <c r="E36" s="34" t="s">
         <v>125</v>
       </c>
@@ -13573,7 +14936,7 @@
     <row r="37" spans="1:20" ht="13.15" customHeight="1">
       <c r="B37" s="278"/>
       <c r="C37" s="33"/>
-      <c r="D37" s="603" t="s">
+      <c r="D37" s="607" t="s">
         <v>21</v>
       </c>
       <c r="E37" s="58" t="s">
@@ -13623,7 +14986,7 @@
     <row r="38" spans="1:20" ht="13.15" customHeight="1">
       <c r="B38" s="278"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="604"/>
+      <c r="D38" s="608"/>
       <c r="E38" s="28" t="s">
         <v>23</v>
       </c>
@@ -13673,7 +15036,7 @@
     <row r="39" spans="1:20" s="37" customFormat="1" ht="13.15" customHeight="1">
       <c r="B39" s="278"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="605"/>
+      <c r="D39" s="609"/>
       <c r="E39" s="34" t="s">
         <v>126</v>
       </c>
@@ -13761,10 +15124,10 @@
     <row r="41" spans="1:20" ht="13.15" customHeight="1">
       <c r="B41" s="278"/>
       <c r="C41" s="33"/>
-      <c r="D41" s="621" t="s">
+      <c r="D41" s="625" t="s">
         <v>264</v>
       </c>
-      <c r="E41" s="622"/>
+      <c r="E41" s="626"/>
       <c r="F41" s="31" t="s">
         <v>262</v>
       </c>
@@ -13810,8 +15173,8 @@
     <row r="42" spans="1:20" ht="13.15" customHeight="1">
       <c r="B42" s="278"/>
       <c r="C42" s="33"/>
-      <c r="D42" s="623"/>
-      <c r="E42" s="624"/>
+      <c r="D42" s="627"/>
+      <c r="E42" s="628"/>
       <c r="F42" s="31" t="s">
         <v>263</v>
       </c>
@@ -13858,10 +15221,10 @@
     <row r="43" spans="1:20" ht="13.15" customHeight="1">
       <c r="B43" s="278"/>
       <c r="C43" s="33"/>
-      <c r="D43" s="596" t="s">
+      <c r="D43" s="600" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="597"/>
+      <c r="E43" s="601"/>
       <c r="F43" s="31"/>
       <c r="G43" s="338">
         <v>29</v>
@@ -13905,10 +15268,10 @@
     <row r="44" spans="1:20" ht="13.15" customHeight="1">
       <c r="B44" s="278"/>
       <c r="C44" s="33"/>
-      <c r="D44" s="596" t="s">
+      <c r="D44" s="600" t="s">
         <v>26</v>
       </c>
-      <c r="E44" s="597"/>
+      <c r="E44" s="601"/>
       <c r="F44" s="31"/>
       <c r="G44" s="338">
         <v>30</v>
@@ -13952,10 +15315,10 @@
     <row r="45" spans="1:20" ht="13.15" customHeight="1">
       <c r="B45" s="278"/>
       <c r="C45" s="33"/>
-      <c r="D45" s="596" t="s">
+      <c r="D45" s="600" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="597"/>
+      <c r="E45" s="601"/>
       <c r="F45" s="31"/>
       <c r="G45" s="338">
         <v>31</v>
@@ -14161,7 +15524,7 @@
     <row r="50" spans="1:20">
       <c r="B50" s="278"/>
       <c r="C50" s="33"/>
-      <c r="D50" s="603" t="s">
+      <c r="D50" s="607" t="s">
         <v>34</v>
       </c>
       <c r="E50" s="74" t="s">
@@ -14211,7 +15574,7 @@
     <row r="51" spans="1:20">
       <c r="B51" s="278"/>
       <c r="C51" s="33"/>
-      <c r="D51" s="604"/>
+      <c r="D51" s="608"/>
       <c r="E51" s="74" t="s">
         <v>36</v>
       </c>
@@ -14259,7 +15622,7 @@
     <row r="52" spans="1:20">
       <c r="B52" s="278"/>
       <c r="C52" s="33"/>
-      <c r="D52" s="604"/>
+      <c r="D52" s="608"/>
       <c r="E52" s="74" t="s">
         <v>37</v>
       </c>
@@ -14307,7 +15670,7 @@
     <row r="53" spans="1:20">
       <c r="B53" s="278"/>
       <c r="C53" s="33"/>
-      <c r="D53" s="604"/>
+      <c r="D53" s="608"/>
       <c r="E53" s="74" t="s">
         <v>38</v>
       </c>
@@ -14355,7 +15718,7 @@
     <row r="54" spans="1:20" s="37" customFormat="1" ht="13.5" thickBot="1">
       <c r="B54" s="278"/>
       <c r="C54" s="84"/>
-      <c r="D54" s="605"/>
+      <c r="D54" s="609"/>
       <c r="E54" s="170" t="s">
         <v>128</v>
       </c>
@@ -14518,7 +15881,7 @@
     <row r="58" spans="1:20">
       <c r="B58" s="278"/>
       <c r="C58" s="33"/>
-      <c r="D58" s="607" t="s">
+      <c r="D58" s="611" t="s">
         <v>43</v>
       </c>
       <c r="E58" s="86" t="s">
@@ -14568,7 +15931,7 @@
     <row r="59" spans="1:20">
       <c r="B59" s="278"/>
       <c r="C59" s="33"/>
-      <c r="D59" s="607"/>
+      <c r="D59" s="611"/>
       <c r="E59" s="86" t="s">
         <v>45</v>
       </c>
@@ -14617,7 +15980,7 @@
       <c r="A60" s="285"/>
       <c r="B60" s="278"/>
       <c r="C60" s="33"/>
-      <c r="D60" s="607"/>
+      <c r="D60" s="611"/>
       <c r="E60" s="34" t="s">
         <v>87</v>
       </c>
@@ -14682,7 +16045,7 @@
     <row r="61" spans="1:20">
       <c r="B61" s="278"/>
       <c r="C61" s="230"/>
-      <c r="D61" s="607"/>
+      <c r="D61" s="611"/>
       <c r="E61" s="86" t="s">
         <v>104</v>
       </c>
@@ -14730,7 +16093,7 @@
     <row r="62" spans="1:20">
       <c r="B62" s="278"/>
       <c r="C62" s="33"/>
-      <c r="D62" s="607"/>
+      <c r="D62" s="611"/>
       <c r="E62" s="86" t="s">
         <v>103</v>
       </c>
@@ -14864,11 +16227,11 @@
     <row r="65" spans="1:20">
       <c r="B65" s="278"/>
       <c r="C65" s="33"/>
-      <c r="D65" s="595" t="s">
+      <c r="D65" s="599" t="s">
         <v>94</v>
       </c>
-      <c r="E65" s="595"/>
-      <c r="F65" s="595"/>
+      <c r="E65" s="599"/>
+      <c r="F65" s="599"/>
       <c r="G65" s="338">
         <v>46</v>
       </c>
@@ -14911,11 +16274,11 @@
     <row r="66" spans="1:20">
       <c r="B66" s="278"/>
       <c r="C66" s="33"/>
-      <c r="D66" s="595" t="s">
+      <c r="D66" s="599" t="s">
         <v>95</v>
       </c>
-      <c r="E66" s="595"/>
-      <c r="F66" s="595"/>
+      <c r="E66" s="599"/>
+      <c r="F66" s="599"/>
       <c r="G66" s="338">
         <v>47</v>
       </c>
@@ -14981,11 +16344,11 @@
     <row r="68" spans="1:20">
       <c r="B68" s="278"/>
       <c r="C68" s="33"/>
-      <c r="D68" s="595" t="s">
+      <c r="D68" s="599" t="s">
         <v>120</v>
       </c>
-      <c r="E68" s="595"/>
-      <c r="F68" s="595"/>
+      <c r="E68" s="599"/>
+      <c r="F68" s="599"/>
       <c r="G68" s="338">
         <v>48</v>
       </c>
@@ -15028,11 +16391,11 @@
     <row r="69" spans="1:20">
       <c r="B69" s="278"/>
       <c r="C69" s="33"/>
-      <c r="D69" s="595" t="s">
+      <c r="D69" s="599" t="s">
         <v>122</v>
       </c>
-      <c r="E69" s="595"/>
-      <c r="F69" s="595"/>
+      <c r="E69" s="599"/>
+      <c r="F69" s="599"/>
       <c r="G69" s="338">
         <v>49</v>
       </c>
@@ -15075,11 +16438,11 @@
     <row r="70" spans="1:20">
       <c r="B70" s="278"/>
       <c r="C70" s="33"/>
-      <c r="D70" s="595" t="s">
+      <c r="D70" s="599" t="s">
         <v>123</v>
       </c>
-      <c r="E70" s="595"/>
-      <c r="F70" s="595"/>
+      <c r="E70" s="599"/>
+      <c r="F70" s="599"/>
       <c r="G70" s="338">
         <v>50</v>
       </c>
@@ -15145,7 +16508,7 @@
     <row r="72" spans="1:20">
       <c r="B72" s="278"/>
       <c r="C72" s="33"/>
-      <c r="D72" s="608" t="s">
+      <c r="D72" s="612" t="s">
         <v>46</v>
       </c>
       <c r="E72" s="98" t="s">
@@ -15194,7 +16557,7 @@
     <row r="73" spans="1:20">
       <c r="B73" s="278"/>
       <c r="C73" s="33"/>
-      <c r="D73" s="608"/>
+      <c r="D73" s="612"/>
       <c r="E73" s="98" t="s">
         <v>105</v>
       </c>
@@ -15242,7 +16605,7 @@
     <row r="74" spans="1:20">
       <c r="B74" s="278"/>
       <c r="C74" s="33"/>
-      <c r="D74" s="608"/>
+      <c r="D74" s="612"/>
       <c r="E74" s="98" t="s">
         <v>48</v>
       </c>
@@ -15290,7 +16653,7 @@
     <row r="75" spans="1:20">
       <c r="B75" s="278"/>
       <c r="C75" s="33"/>
-      <c r="D75" s="608"/>
+      <c r="D75" s="612"/>
       <c r="E75" s="98" t="s">
         <v>49</v>
       </c>
@@ -15338,7 +16701,7 @@
     <row r="76" spans="1:20">
       <c r="B76" s="278"/>
       <c r="C76" s="33"/>
-      <c r="D76" s="608"/>
+      <c r="D76" s="612"/>
       <c r="E76" s="98" t="s">
         <v>50</v>
       </c>
@@ -15386,7 +16749,7 @@
     <row r="77" spans="1:20">
       <c r="B77" s="278"/>
       <c r="C77" s="33"/>
-      <c r="D77" s="608"/>
+      <c r="D77" s="612"/>
       <c r="E77" s="74" t="s">
         <v>51</v>
       </c>
@@ -15565,7 +16928,7 @@
     <row r="80" spans="1:20">
       <c r="B80" s="278"/>
       <c r="C80" s="33"/>
-      <c r="D80" s="603" t="s">
+      <c r="D80" s="607" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="98" t="s">
@@ -15614,7 +16977,7 @@
     <row r="81" spans="2:20">
       <c r="B81" s="278"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="604"/>
+      <c r="D81" s="608"/>
       <c r="E81" s="98" t="s">
         <v>201</v>
       </c>
@@ -15662,7 +17025,7 @@
     <row r="82" spans="2:20">
       <c r="B82" s="278"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="604"/>
+      <c r="D82" s="608"/>
       <c r="E82" s="98" t="s">
         <v>202</v>
       </c>
@@ -15710,7 +17073,7 @@
     <row r="83" spans="2:20">
       <c r="B83" s="278"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="605"/>
+      <c r="D83" s="609"/>
       <c r="E83" s="98" t="s">
         <v>203</v>
       </c>
@@ -15823,13 +17186,13 @@
     <row r="85" spans="2:20" ht="13.15" customHeight="1">
       <c r="B85" s="278"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="606" t="s">
+      <c r="D85" s="610" t="s">
         <v>53</v>
       </c>
-      <c r="E85" s="596" t="s">
+      <c r="E85" s="600" t="s">
         <v>206</v>
       </c>
-      <c r="F85" s="597"/>
+      <c r="F85" s="601"/>
       <c r="G85" s="338">
         <f t="shared" si="10"/>
         <v>64</v>
@@ -15873,7 +17236,7 @@
     <row r="86" spans="2:20">
       <c r="B86" s="278"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="606"/>
+      <c r="D86" s="610"/>
       <c r="E86" s="98" t="s">
         <v>54</v>
       </c>
@@ -15921,7 +17284,7 @@
     <row r="87" spans="2:20">
       <c r="B87" s="278"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="606"/>
+      <c r="D87" s="610"/>
       <c r="E87" s="34" t="s">
         <v>134</v>
       </c>
@@ -15986,7 +17349,7 @@
     <row r="88" spans="2:20">
       <c r="B88" s="278"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="606" t="s">
+      <c r="D88" s="610" t="s">
         <v>55</v>
       </c>
       <c r="E88" s="98" t="s">
@@ -16036,7 +17399,7 @@
     <row r="89" spans="2:20">
       <c r="B89" s="278"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="606"/>
+      <c r="D89" s="610"/>
       <c r="E89" s="98" t="s">
         <v>56</v>
       </c>
@@ -16084,7 +17447,7 @@
     <row r="90" spans="2:20">
       <c r="B90" s="278"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="606"/>
+      <c r="D90" s="610"/>
       <c r="E90" s="98" t="s">
         <v>200</v>
       </c>
@@ -16132,7 +17495,7 @@
     <row r="91" spans="2:20">
       <c r="B91" s="278"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="603" t="s">
+      <c r="D91" s="607" t="s">
         <v>57</v>
       </c>
       <c r="E91" s="98" t="s">
@@ -16182,7 +17545,7 @@
     <row r="92" spans="2:20" s="102" customFormat="1">
       <c r="B92" s="278"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="604"/>
+      <c r="D92" s="608"/>
       <c r="E92" s="98" t="s">
         <v>58</v>
       </c>
@@ -16230,7 +17593,7 @@
     <row r="93" spans="2:20">
       <c r="B93" s="278"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="605"/>
+      <c r="D93" s="609"/>
       <c r="E93" s="98" t="s">
         <v>207</v>
       </c>
@@ -16343,11 +17706,11 @@
     <row r="95" spans="2:20">
       <c r="B95" s="278"/>
       <c r="C95" s="84"/>
-      <c r="D95" s="598" t="s">
+      <c r="D95" s="602" t="s">
         <v>59</v>
       </c>
-      <c r="E95" s="599"/>
-      <c r="F95" s="600"/>
+      <c r="E95" s="603"/>
+      <c r="F95" s="604"/>
       <c r="G95" s="338">
         <f t="shared" si="10"/>
         <v>74</v>
@@ -17730,8 +19093,8 @@
         <v>79</v>
       </c>
       <c r="D125" s="148"/>
-      <c r="E125" s="601"/>
-      <c r="F125" s="602"/>
+      <c r="E125" s="605"/>
+      <c r="F125" s="606"/>
       <c r="G125" s="338"/>
       <c r="H125" s="450"/>
       <c r="I125" s="451"/>
@@ -20255,18 +21618,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8629DAB4-A91A-4D1E-92A9-9AE2403D6050}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>394</v>
       </c>
@@ -20274,7 +21638,7 @@
         <v>11199</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -20282,7 +21646,7 @@
         <v>5938</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>415</v>
       </c>
@@ -20290,21 +21654,21 @@
         <v>10211</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>416</v>
       </c>
-      <c r="B4" s="655">
+      <c r="B4" s="595">
         <f>B3/B1</f>
         <v>0.91177783730690243</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="657" t="s">
+    <row r="8" spans="1:13">
+      <c r="A8" s="597" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>393</v>
       </c>
@@ -20312,48 +21676,126 @@
         <v>8731</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>395</v>
       </c>
       <c r="B10">
         <v>8647</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="K10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>396</v>
       </c>
-      <c r="B11" s="655">
+      <c r="B11" s="595">
         <f>B10/B9</f>
         <v>0.99037910892223113</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="J11" t="s">
+        <v>427</v>
+      </c>
+      <c r="K11" s="660">
+        <v>0.02</v>
+      </c>
+      <c r="L11" s="660">
+        <f>K11/K16</f>
+        <v>5.8139534883720929E-3</v>
+      </c>
+      <c r="M11" s="660">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>390</v>
       </c>
       <c r="B12">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="J12" t="s">
+        <v>429</v>
+      </c>
+      <c r="K12" s="660">
+        <v>0.7</v>
+      </c>
+      <c r="L12" s="660">
+        <f>K12/K16</f>
+        <v>0.20348837209302326</v>
+      </c>
+      <c r="M12" s="660">
+        <f>M11+L12</f>
+        <v>0.21348837209302327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="656">
+      <c r="B13" s="596">
         <f>B12/B1</f>
         <v>3.8396285382623447E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" s="656"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" s="656"/>
+      <c r="J13" t="s">
+        <v>403</v>
+      </c>
+      <c r="K13" s="660">
+        <v>0.83</v>
+      </c>
+      <c r="L13" s="660">
+        <f>K13/K16</f>
+        <v>0.24127906976744184</v>
+      </c>
+      <c r="M13" s="660">
+        <f>M12+L13</f>
+        <v>0.45476744186046514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="596"/>
+      <c r="J14" t="s">
+        <v>430</v>
+      </c>
+      <c r="K14" s="660">
+        <v>0.93</v>
+      </c>
+      <c r="L14" s="660">
+        <f>K14/K16</f>
+        <v>0.27034883720930236</v>
+      </c>
+      <c r="M14" s="660">
+        <f>M13+L14</f>
+        <v>0.7251162790697675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="596"/>
+      <c r="J15" t="s">
+        <v>400</v>
+      </c>
+      <c r="K15" s="660">
+        <v>0.96</v>
+      </c>
+      <c r="L15" s="660">
+        <f>K15/K16</f>
+        <v>0.27906976744186046</v>
+      </c>
+      <c r="M15" s="660">
+        <f>M14+L15</f>
+        <v>1.0041860465116279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="K16" s="660">
+        <f>SUM(K11:K15)</f>
+        <v>3.44</v>
+      </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="657" t="s">
+      <c r="A17" s="597" t="s">
         <v>397</v>
       </c>
     </row>
@@ -20361,7 +21803,7 @@
       <c r="A18" t="s">
         <v>398</v>
       </c>
-      <c r="B18" s="658">
+      <c r="B18" s="598">
         <v>8.997685185185185E-2</v>
       </c>
     </row>
@@ -20369,24 +21811,24 @@
       <c r="A19" t="s">
         <v>399</v>
       </c>
-      <c r="B19" s="658">
-        <v>9.375E-2</v>
+      <c r="B19" s="598">
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>402</v>
       </c>
-      <c r="B20" s="655">
+      <c r="B20" s="595">
         <f>B19/B18</f>
-        <v>1.0419346539747878</v>
+        <v>1.0805248263442244</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>400</v>
       </c>
-      <c r="B22" s="658">
+      <c r="B22" s="598">
         <v>7.6006944444444446E-2</v>
       </c>
     </row>
@@ -20394,7 +21836,7 @@
       <c r="A23" t="s">
         <v>401</v>
       </c>
-      <c r="B23" s="658">
+      <c r="B23" s="598">
         <v>7.2916666666666671E-2</v>
       </c>
     </row>
@@ -20402,7 +21844,7 @@
       <c r="A24" t="s">
         <v>402</v>
       </c>
-      <c r="B24" s="655">
+      <c r="B24" s="595">
         <f>B23/B22</f>
         <v>0.9593421653723162</v>
       </c>
@@ -20411,7 +21853,7 @@
       <c r="A26" t="s">
         <v>403</v>
       </c>
-      <c r="B26" s="658">
+      <c r="B26" s="598">
         <v>5.0405092592592592E-2</v>
       </c>
     </row>
@@ -20419,7 +21861,7 @@
       <c r="A27" t="s">
         <v>404</v>
       </c>
-      <c r="B27" s="658">
+      <c r="B27" s="598">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -20427,13 +21869,13 @@
       <c r="A28" t="s">
         <v>402</v>
       </c>
-      <c r="B28" s="655">
+      <c r="B28" s="595">
         <f>B27/B26</f>
         <v>0.82663605051664746</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="657" t="s">
+      <c r="A31" s="597" t="s">
         <v>405</v>
       </c>
     </row>
@@ -20445,43 +21887,99 @@
         <v>4423</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>407</v>
       </c>
-      <c r="B33" s="655">
+      <c r="B33" s="595">
         <f>B32/B1</f>
         <v>0.39494597731940351</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="657" t="s">
+    <row r="36" spans="1:10">
+      <c r="A36" s="597" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>409</v>
       </c>
       <c r="B37">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="G37">
+        <v>85</v>
+      </c>
+      <c r="H37">
+        <v>73</v>
+      </c>
+      <c r="I37">
+        <f>G37*H37</f>
+        <v>6205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>410</v>
       </c>
-      <c r="B38" s="656">
+      <c r="B38" s="596">
         <f>B37/B2</f>
         <v>9.2623779050185241E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="657" t="s">
+      <c r="G38">
+        <v>90</v>
+      </c>
+      <c r="H38">
+        <v>16</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38:I40" si="0">G38*H38</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="G39">
+        <v>100</v>
+      </c>
+      <c r="H39">
+        <v>26</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="G40">
+        <v>60</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="597" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="H41">
+        <f>SUM(H37:H40)</f>
+        <v>116</v>
+      </c>
+      <c r="I41">
+        <f>SUM(I37:I40)</f>
+        <v>10305</v>
+      </c>
+      <c r="J41">
+        <f>I41/H41</f>
+        <v>88.83620689655173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>413</v>
       </c>
@@ -20489,21 +21987,21 @@
         <v>4479</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>414</v>
       </c>
-      <c r="B43" s="655">
+      <c r="B43" s="595">
         <f>B42/B1</f>
         <v>0.39994642378783818</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="657" t="s">
+    <row r="46" spans="1:10">
+      <c r="A46" s="597" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>418</v>
       </c>
@@ -20511,7 +22009,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>419</v>
       </c>
@@ -20519,14 +22017,58 @@
         <v>427</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>420</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="597" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>422</v>
+      </c>
+      <c r="B53">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>423</v>
+      </c>
+      <c r="B54">
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="597" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>425</v>
+      </c>
+      <c r="B58">
+        <v>4748427</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>426</v>
+      </c>
+      <c r="B59" s="659">
+        <f>B58/B3</f>
+        <v>465.0305552835178</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21157,10 +22699,10 @@
       </c>
       <c r="B4" s="505"/>
       <c r="C4" s="506"/>
-      <c r="D4" s="645" t="s">
+      <c r="D4" s="649" t="s">
         <v>334</v>
       </c>
-      <c r="E4" s="645"/>
+      <c r="E4" s="649"/>
     </row>
     <row r="5" spans="1:31" ht="26.25" customHeight="1">
       <c r="A5" s="504" t="s">
@@ -21168,10 +22710,10 @@
       </c>
       <c r="B5" s="505"/>
       <c r="C5" s="506"/>
-      <c r="D5" s="645" t="s">
+      <c r="D5" s="649" t="s">
         <v>335</v>
       </c>
-      <c r="E5" s="645"/>
+      <c r="E5" s="649"/>
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="507"/>
@@ -21203,12 +22745,12 @@
       <c r="A8" s="515" t="s">
         <v>337</v>
       </c>
-      <c r="B8" s="646" t="s">
+      <c r="B8" s="650" t="s">
         <v>338</v>
       </c>
-      <c r="C8" s="647"/>
-      <c r="D8" s="647"/>
-      <c r="E8" s="648"/>
+      <c r="C8" s="651"/>
+      <c r="D8" s="651"/>
+      <c r="E8" s="652"/>
       <c r="F8" s="515"/>
       <c r="G8" s="516" t="s">
         <v>339</v>
@@ -21349,10 +22891,10 @@
     <row r="11" spans="1:31" ht="30" customHeight="1">
       <c r="A11" s="522"/>
       <c r="B11" s="510"/>
-      <c r="C11" s="649" t="s">
+      <c r="C11" s="653" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="652" t="s">
+      <c r="D11" s="656" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="532">
@@ -21440,8 +22982,8 @@
     <row r="12" spans="1:31" ht="30" customHeight="1">
       <c r="A12" s="522"/>
       <c r="B12" s="510"/>
-      <c r="C12" s="650"/>
-      <c r="D12" s="653"/>
+      <c r="C12" s="654"/>
+      <c r="D12" s="657"/>
       <c r="E12" s="532">
         <v>20</v>
       </c>
@@ -21527,8 +23069,8 @@
     <row r="13" spans="1:31" ht="30" customHeight="1">
       <c r="A13" s="522"/>
       <c r="B13" s="510"/>
-      <c r="C13" s="650"/>
-      <c r="D13" s="653"/>
+      <c r="C13" s="654"/>
+      <c r="D13" s="657"/>
       <c r="E13" s="532">
         <v>30</v>
       </c>
@@ -21614,8 +23156,8 @@
     <row r="14" spans="1:31" ht="30" customHeight="1">
       <c r="A14" s="522"/>
       <c r="B14" s="510"/>
-      <c r="C14" s="650"/>
-      <c r="D14" s="653"/>
+      <c r="C14" s="654"/>
+      <c r="D14" s="657"/>
       <c r="E14" s="532">
         <v>40</v>
       </c>
@@ -21701,8 +23243,8 @@
     <row r="15" spans="1:31" ht="30" customHeight="1">
       <c r="A15" s="522"/>
       <c r="B15" s="510"/>
-      <c r="C15" s="650"/>
-      <c r="D15" s="653"/>
+      <c r="C15" s="654"/>
+      <c r="D15" s="657"/>
       <c r="E15" s="532">
         <v>50</v>
       </c>
@@ -21788,8 +23330,8 @@
     <row r="16" spans="1:31" ht="30" customHeight="1">
       <c r="A16" s="522"/>
       <c r="B16" s="510"/>
-      <c r="C16" s="650"/>
-      <c r="D16" s="653"/>
+      <c r="C16" s="654"/>
+      <c r="D16" s="657"/>
       <c r="E16" s="532">
         <v>60</v>
       </c>
@@ -21875,8 +23417,8 @@
     <row r="17" spans="1:31" ht="30" customHeight="1">
       <c r="A17" s="522"/>
       <c r="B17" s="510"/>
-      <c r="C17" s="650"/>
-      <c r="D17" s="653"/>
+      <c r="C17" s="654"/>
+      <c r="D17" s="657"/>
       <c r="E17" s="532">
         <v>70</v>
       </c>
@@ -21962,8 +23504,8 @@
     <row r="18" spans="1:31" ht="30" customHeight="1">
       <c r="A18" s="522"/>
       <c r="B18" s="510"/>
-      <c r="C18" s="650"/>
-      <c r="D18" s="653"/>
+      <c r="C18" s="654"/>
+      <c r="D18" s="657"/>
       <c r="E18" s="532">
         <v>80</v>
       </c>
@@ -22049,8 +23591,8 @@
     <row r="19" spans="1:31" ht="30" customHeight="1">
       <c r="A19" s="522"/>
       <c r="B19" s="510"/>
-      <c r="C19" s="650"/>
-      <c r="D19" s="653"/>
+      <c r="C19" s="654"/>
+      <c r="D19" s="657"/>
       <c r="E19" s="532">
         <v>90</v>
       </c>
@@ -22136,8 +23678,8 @@
     <row r="20" spans="1:31" ht="30" customHeight="1">
       <c r="A20" s="522"/>
       <c r="B20" s="510"/>
-      <c r="C20" s="650"/>
-      <c r="D20" s="653"/>
+      <c r="C20" s="654"/>
+      <c r="D20" s="657"/>
       <c r="E20" s="532">
         <v>100</v>
       </c>
@@ -22223,8 +23765,8 @@
     <row r="21" spans="1:31" ht="30" customHeight="1">
       <c r="A21" s="522"/>
       <c r="B21" s="510"/>
-      <c r="C21" s="650"/>
-      <c r="D21" s="653"/>
+      <c r="C21" s="654"/>
+      <c r="D21" s="657"/>
       <c r="E21" s="536" t="s">
         <v>19</v>
       </c>
@@ -22260,8 +23802,8 @@
     <row r="22" spans="1:31" ht="30" customHeight="1">
       <c r="A22" s="522"/>
       <c r="B22" s="510"/>
-      <c r="C22" s="650"/>
-      <c r="D22" s="654"/>
+      <c r="C22" s="654"/>
+      <c r="D22" s="658"/>
       <c r="E22" s="539" t="s">
         <v>20</v>
       </c>
@@ -22347,7 +23889,7 @@
     <row r="23" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A23" s="541"/>
       <c r="B23" s="542"/>
-      <c r="C23" s="651"/>
+      <c r="C23" s="655"/>
       <c r="D23" s="543" t="s">
         <v>364</v>
       </c>
@@ -22436,13 +23978,13 @@
     <row r="24" spans="1:31" ht="30" customHeight="1">
       <c r="A24" s="522"/>
       <c r="B24" s="510"/>
-      <c r="C24" s="640" t="s">
+      <c r="C24" s="644" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="643" t="s">
+      <c r="D24" s="647" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="644"/>
+      <c r="E24" s="648"/>
       <c r="F24" s="526">
         <v>14</v>
       </c>
@@ -22525,7 +24067,7 @@
     <row r="25" spans="1:31" ht="30" customHeight="1">
       <c r="A25" s="522"/>
       <c r="B25" s="510"/>
-      <c r="C25" s="641"/>
+      <c r="C25" s="645"/>
       <c r="D25" s="548" t="s">
         <v>23</v>
       </c>
@@ -22614,7 +24156,7 @@
     <row r="26" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A26" s="541"/>
       <c r="B26" s="542"/>
-      <c r="C26" s="642"/>
+      <c r="C26" s="646"/>
       <c r="D26" s="543" t="s">
         <v>366</v>
       </c>
@@ -22703,10 +24245,10 @@
     <row r="27" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A27" s="541"/>
       <c r="B27" s="542"/>
-      <c r="C27" s="631" t="s">
+      <c r="C27" s="635" t="s">
         <v>368</v>
       </c>
-      <c r="D27" s="632"/>
+      <c r="D27" s="636"/>
       <c r="E27" s="549" t="s">
         <v>369</v>
       </c>
@@ -22827,10 +24369,10 @@
     <row r="29" spans="1:31" ht="30" customHeight="1">
       <c r="A29" s="522"/>
       <c r="B29" s="510"/>
-      <c r="C29" s="633" t="s">
+      <c r="C29" s="637" t="s">
         <v>371</v>
       </c>
-      <c r="D29" s="634"/>
+      <c r="D29" s="638"/>
       <c r="E29" s="539" t="s">
         <v>372</v>
       </c>
@@ -22916,8 +24458,8 @@
     <row r="30" spans="1:31" ht="30" customHeight="1">
       <c r="A30" s="522"/>
       <c r="B30" s="510"/>
-      <c r="C30" s="635"/>
-      <c r="D30" s="636"/>
+      <c r="C30" s="639"/>
+      <c r="D30" s="640"/>
       <c r="E30" s="539" t="s">
         <v>373</v>
       </c>
@@ -23003,10 +24545,10 @@
     <row r="31" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A31" s="541"/>
       <c r="B31" s="542"/>
-      <c r="C31" s="637" t="s">
+      <c r="C31" s="641" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="638"/>
+      <c r="D31" s="642"/>
       <c r="E31" s="555"/>
       <c r="F31" s="527">
         <v>20</v>
@@ -23090,10 +24632,10 @@
     <row r="32" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A32" s="541"/>
       <c r="B32" s="542"/>
-      <c r="C32" s="637" t="s">
+      <c r="C32" s="641" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="638"/>
+      <c r="D32" s="642"/>
       <c r="E32" s="555"/>
       <c r="F32" s="527">
         <v>21</v>
@@ -23127,10 +24669,10 @@
     <row r="33" spans="1:31" s="557" customFormat="1" ht="30" customHeight="1">
       <c r="A33" s="541"/>
       <c r="B33" s="542"/>
-      <c r="C33" s="637" t="s">
+      <c r="C33" s="641" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="638"/>
+      <c r="D33" s="642"/>
       <c r="E33" s="555"/>
       <c r="F33" s="527">
         <v>22</v>
@@ -23164,10 +24706,10 @@
     <row r="34" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1">
       <c r="A34" s="541"/>
       <c r="B34" s="558"/>
-      <c r="C34" s="631" t="s">
+      <c r="C34" s="635" t="s">
         <v>374</v>
       </c>
-      <c r="D34" s="639"/>
+      <c r="D34" s="643"/>
       <c r="E34" s="549" t="s">
         <v>375</v>
       </c>
@@ -23202,11 +24744,11 @@
     </row>
     <row r="35" spans="1:31" s="547" customFormat="1" ht="30" customHeight="1" thickBot="1">
       <c r="A35" s="559"/>
-      <c r="B35" s="625" t="s">
+      <c r="B35" s="629" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="626"/>
-      <c r="D35" s="627"/>
+      <c r="C35" s="630"/>
+      <c r="D35" s="631"/>
       <c r="E35" s="560" t="s">
         <v>377</v>
       </c>
@@ -23329,7 +24871,7 @@
     <row r="37" spans="1:31" ht="30" customHeight="1">
       <c r="A37" s="563"/>
       <c r="B37" s="571"/>
-      <c r="C37" s="628" t="s">
+      <c r="C37" s="632" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="572" t="s">
@@ -23418,7 +24960,7 @@
     <row r="38" spans="1:31" ht="30" customHeight="1">
       <c r="A38" s="563"/>
       <c r="B38" s="571"/>
-      <c r="C38" s="629"/>
+      <c r="C38" s="633"/>
       <c r="D38" s="572" t="s">
         <v>36</v>
       </c>
@@ -23505,7 +25047,7 @@
     <row r="39" spans="1:31" ht="30" customHeight="1">
       <c r="A39" s="563"/>
       <c r="B39" s="571"/>
-      <c r="C39" s="629"/>
+      <c r="C39" s="633"/>
       <c r="D39" s="572" t="s">
         <v>37</v>
       </c>
@@ -23592,7 +25134,7 @@
     <row r="40" spans="1:31" ht="30" customHeight="1">
       <c r="A40" s="563"/>
       <c r="B40" s="571"/>
-      <c r="C40" s="629"/>
+      <c r="C40" s="633"/>
       <c r="D40" s="572" t="s">
         <v>38</v>
       </c>
@@ -23629,7 +25171,7 @@
     <row r="41" spans="1:31" ht="30" customHeight="1" thickBot="1">
       <c r="A41" s="576"/>
       <c r="B41" s="577"/>
-      <c r="C41" s="630"/>
+      <c r="C41" s="634"/>
       <c r="D41" s="578" t="s">
         <v>379</v>
       </c>

</xml_diff>